<commit_message>
set alcohol, coffee and tea to status quo in all scenarios, correct portion error for meat and add losses to fruit/veg/fish
</commit_message>
<xml_diff>
--- a/inst/items_conc.xlsx
+++ b/inst/items_conc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\str\Desktop\WWF\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F2780D-35B6-4DE8-A281-D594CB10FE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD0A401-62E8-49AC-95BE-C667A8CC545A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="concordance" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5984" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6043" uniqueCount="676">
   <si>
     <t>comm_code</t>
   </si>
@@ -1892,9 +1892,6 @@
     <t>&lt;= 3/week</t>
   </si>
   <si>
-    <t>300 – 450</t>
-  </si>
-  <si>
     <t>1-2</t>
   </si>
   <si>
@@ -1907,9 +1904,6 @@
     <t>100 - 200</t>
   </si>
   <si>
-    <t>&lt;=3-4</t>
-  </si>
-  <si>
     <t>0 - 300</t>
   </si>
   <si>
@@ -2061,6 +2055,24 @@
   </si>
   <si>
     <t>portion size/subgroup</t>
+  </si>
+  <si>
+    <t>assumed same as fruits</t>
+  </si>
+  <si>
+    <t>1 - average edible flesh share from https://www.fao.org/3/T0219E/T0219E01.htm</t>
+  </si>
+  <si>
+    <t>Spirituosen</t>
+  </si>
+  <si>
+    <t>Spirits</t>
+  </si>
+  <si>
+    <t>Bier und Most</t>
+  </si>
+  <si>
+    <t>Beer and cider</t>
   </si>
 </sst>
 </file>
@@ -2069,7 +2081,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -2748,7 +2760,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -2829,18 +2841,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2848,7 +2848,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="41" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2866,7 +2866,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2886,6 +2886,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3245,31 +3259,31 @@
   <dimension ref="A1:Q124"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="N43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P1" sqref="P1"/>
+      <selection pane="bottomRight" activeCell="O91" sqref="O91:P94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="12.07421875" customWidth="1"/>
-    <col min="3" max="3" width="34.3046875" customWidth="1"/>
-    <col min="4" max="4" width="16.84375" customWidth="1"/>
-    <col min="5" max="5" width="16.23046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.07421875" customWidth="1"/>
-    <col min="7" max="7" width="11.4609375" customWidth="1"/>
-    <col min="8" max="8" width="31.15234375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.23046875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="29.84375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="31.3046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.3046875" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.3046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.3046875" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.3046875" style="14" customWidth="1"/>
-    <col min="16" max="16" width="31.3046875" style="33" customWidth="1"/>
-    <col min="17" max="17" width="31.15234375" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="29.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="31.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.28515625" style="14" customWidth="1"/>
+    <col min="16" max="16" width="31.28515625" style="33" customWidth="1"/>
+    <col min="17" max="17" width="31.140625" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -3319,7 +3333,7 @@
         <v>602</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="Q1" s="14" t="s">
         <v>365</v>
@@ -4212,7 +4226,7 @@
         <v>611</v>
       </c>
       <c r="P18" s="33" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="Q18" s="14" t="s">
         <v>383</v>
@@ -4265,7 +4279,7 @@
         <v>611</v>
       </c>
       <c r="P19" s="33" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="Q19" s="14" t="s">
         <v>383</v>
@@ -4318,7 +4332,7 @@
         <v>611</v>
       </c>
       <c r="P20" s="33" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="Q20" s="14" t="s">
         <v>383</v>
@@ -4424,7 +4438,7 @@
         <v>611</v>
       </c>
       <c r="P22" s="33" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="Q22" s="14" t="s">
         <v>382</v>
@@ -4473,7 +4487,7 @@
       <c r="N23" s="24" t="s">
         <v>299</v>
       </c>
-      <c r="O23" s="61" t="s">
+      <c r="O23" s="57" t="s">
         <v>609</v>
       </c>
       <c r="P23" s="33" t="s">
@@ -5754,7 +5768,7 @@
         <v>606</v>
       </c>
       <c r="P48" s="33" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="Q48" s="14" t="s">
         <v>106</v>
@@ -7619,10 +7633,10 @@
       <c r="N91" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="O91" s="68" t="s">
+      <c r="O91" s="64" t="s">
         <v>206</v>
       </c>
-      <c r="P91" s="7" t="s">
+      <c r="P91" s="64" t="s">
         <v>205</v>
       </c>
       <c r="Q91" s="14" t="s">
@@ -7672,11 +7686,11 @@
       <c r="N92" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="O92" s="68" t="s">
+      <c r="O92" s="64" t="s">
         <v>206</v>
       </c>
-      <c r="P92" s="7" t="s">
-        <v>208</v>
+      <c r="P92" s="64" t="s">
+        <v>675</v>
       </c>
       <c r="Q92" s="14" t="s">
         <v>206</v>
@@ -7725,11 +7739,11 @@
       <c r="N93" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="O93" s="68" t="s">
-        <v>300</v>
-      </c>
-      <c r="P93" s="68" t="s">
-        <v>300</v>
+      <c r="O93" s="64" t="s">
+        <v>206</v>
+      </c>
+      <c r="P93" s="64" t="s">
+        <v>675</v>
       </c>
       <c r="Q93" s="14" t="s">
         <v>206</v>
@@ -7778,11 +7792,11 @@
       <c r="N94" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="O94" s="68" t="s">
-        <v>300</v>
-      </c>
-      <c r="P94" s="68" t="s">
-        <v>300</v>
+      <c r="O94" s="64" t="s">
+        <v>206</v>
+      </c>
+      <c r="P94" s="64" t="s">
+        <v>673</v>
       </c>
       <c r="Q94" s="14" t="s">
         <v>206</v>
@@ -8980,16 +8994,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD37EB09-49C2-4CB6-B43E-99A45A5F8157}">
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E123" sqref="E123:F123"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E126" sqref="E126:F126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="27.4609375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -9006,10 +9020,10 @@
         <v>602</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -9283,7 +9297,7 @@
       </c>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" s="14" t="s">
         <v>44</v>
       </c>
@@ -9303,7 +9317,7 @@
       </c>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18" s="14" t="s">
         <v>46</v>
       </c>
@@ -9322,7 +9336,7 @@
       </c>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19" s="14" t="s">
         <v>49</v>
       </c>
@@ -9341,7 +9355,7 @@
       </c>
       <c r="F19" s="14"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20" s="14" t="s">
         <v>51</v>
       </c>
@@ -9360,7 +9374,7 @@
       </c>
       <c r="F20" s="14"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" s="14" t="s">
         <v>53</v>
       </c>
@@ -9378,10 +9392,10 @@
         <v>0.5</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="14" t="s">
         <v>55</v>
       </c>
@@ -9400,7 +9414,7 @@
       </c>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" s="14" t="s">
         <v>58</v>
       </c>
@@ -9418,7 +9432,7 @@
       </c>
       <c r="F23" s="14"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="A24" s="14" t="s">
         <v>60</v>
       </c>
@@ -9436,7 +9450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="A25" s="14" t="s">
         <v>62</v>
       </c>
@@ -9454,7 +9468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="A26" s="14" t="s">
         <v>64</v>
       </c>
@@ -9469,7 +9483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27" s="14" t="s">
         <v>66</v>
       </c>
@@ -9487,7 +9501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28" s="14" t="s">
         <v>68</v>
       </c>
@@ -9505,7 +9519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="A29" s="14" t="s">
         <v>70</v>
       </c>
@@ -9520,7 +9534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7">
       <c r="A30" s="14" t="s">
         <v>72</v>
       </c>
@@ -9538,7 +9552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:7">
       <c r="A31" s="14" t="s">
         <v>74</v>
       </c>
@@ -9556,7 +9570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:7">
       <c r="A32" s="14" t="s">
         <v>76</v>
       </c>
@@ -9571,10 +9585,16 @@
         <v>Vegetables and legumes</v>
       </c>
       <c r="E32" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="14" t="s">
         <v>78</v>
       </c>
@@ -9589,10 +9609,16 @@
         <v>Vegetables and legumes</v>
       </c>
       <c r="E33" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="14" t="s">
         <v>80</v>
       </c>
@@ -9607,10 +9633,16 @@
         <v>Vegetables and legumes</v>
       </c>
       <c r="E34" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="14" t="s">
         <v>82</v>
       </c>
@@ -9625,10 +9657,14 @@
         <v>Fruits</v>
       </c>
       <c r="E35" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G35" s="14"/>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="14" t="s">
         <v>84</v>
       </c>
@@ -9643,10 +9679,14 @@
         <v>Fruits</v>
       </c>
       <c r="E36" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G36" s="14"/>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="14" t="s">
         <v>86</v>
       </c>
@@ -9661,10 +9701,14 @@
         <v>Fruits</v>
       </c>
       <c r="E37" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G37" s="14"/>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="14" t="s">
         <v>88</v>
       </c>
@@ -9679,10 +9723,14 @@
         <v>Fruits</v>
       </c>
       <c r="E38" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G38" s="14"/>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="14" t="s">
         <v>90</v>
       </c>
@@ -9697,10 +9745,14 @@
         <v>Fruits</v>
       </c>
       <c r="E39" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G39" s="14"/>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="14" t="s">
         <v>92</v>
       </c>
@@ -9715,10 +9767,14 @@
         <v>Fruits</v>
       </c>
       <c r="E40" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G40" s="14"/>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="14" t="s">
         <v>94</v>
       </c>
@@ -9733,10 +9789,14 @@
         <v>Fruits</v>
       </c>
       <c r="E41" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G41" s="14"/>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="14" t="s">
         <v>96</v>
       </c>
@@ -9751,10 +9811,14 @@
         <v>Fruits</v>
       </c>
       <c r="E42" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G42" s="14"/>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="14" t="s">
         <v>98</v>
       </c>
@@ -9769,10 +9833,14 @@
         <v>Fruits</v>
       </c>
       <c r="E43" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G43" s="14"/>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="14" t="s">
         <v>100</v>
       </c>
@@ -9787,10 +9855,14 @@
         <v>Fruits</v>
       </c>
       <c r="E44" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G44" s="14"/>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="14" t="s">
         <v>102</v>
       </c>
@@ -9805,10 +9877,14 @@
         <v>Fruits</v>
       </c>
       <c r="E45" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G45" s="14"/>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="14" t="s">
         <v>104</v>
       </c>
@@ -9826,10 +9902,10 @@
         <v>0.3</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="14" t="s">
         <v>107</v>
       </c>
@@ -9847,10 +9923,10 @@
         <v>0.2</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="14" t="s">
         <v>109</v>
       </c>
@@ -10628,7 +10704,7 @@
       </c>
       <c r="D94" s="14" t="str">
         <f>VLOOKUP(B94,concordance!$B$2:$Q$124,14,FALSE)</f>
-        <v>Others</v>
+        <v>Alcohol</v>
       </c>
       <c r="E94" s="14">
         <v>0</v>
@@ -10646,7 +10722,7 @@
       </c>
       <c r="D95" s="14" t="str">
         <f>VLOOKUP(B95,concordance!$B$2:$Q$124,14,FALSE)</f>
-        <v>Others</v>
+        <v>Alcohol</v>
       </c>
       <c r="E95" s="14">
         <v>0</v>
@@ -10963,7 +11039,7 @@
         <v>0.34</v>
       </c>
       <c r="F115" s="14" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -10983,7 +11059,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="F116" s="14" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -11003,7 +11079,7 @@
         <v>0.29499999999999998</v>
       </c>
       <c r="F117" s="14" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -11023,7 +11099,7 @@
         <v>0.40500000000000003</v>
       </c>
       <c r="F118" s="14" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -11043,7 +11119,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="F119" s="14" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -11063,7 +11139,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="F120" s="14" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -11116,7 +11192,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="F123" s="14" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -11167,7 +11243,10 @@
         <v>Fish</v>
       </c>
       <c r="E126" s="14">
-        <v>0</v>
+        <v>0.45</v>
+      </c>
+      <c r="F126" s="14" t="s">
+        <v>671</v>
       </c>
     </row>
   </sheetData>
@@ -11183,21 +11262,21 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.23046875" style="14"/>
-    <col min="3" max="3" width="28.23046875" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.23046875" style="14"/>
+    <col min="1" max="2" width="9.28515625" style="14"/>
+    <col min="3" max="3" width="28.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.28515625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="68" t="s">
         <v>373</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="49"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="E1" s="69"/>
+      <c r="F1" s="70"/>
+    </row>
+    <row r="2" spans="1:6" ht="30">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -13729,24 +13808,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F075F6A-B0BD-48B2-B1E2-ACAB1CED68C4}">
   <dimension ref="A1:L124"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J16" sqref="J1:J1048576"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.07421875" style="14" customWidth="1"/>
-    <col min="3" max="3" width="23.53515625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="16.23046875" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.15234375" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.84375" style="36" customWidth="1"/>
-    <col min="7" max="7" width="31.3046875" style="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.53515625" style="33" customWidth="1"/>
-    <col min="9" max="9" width="16.23046875" style="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.3828125" style="33" customWidth="1"/>
-    <col min="11" max="11" width="29.84375" style="36" customWidth="1"/>
-    <col min="12" max="12" width="31.3046875" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" style="36" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" style="33" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.42578125" style="33" customWidth="1"/>
+    <col min="11" max="11" width="29.85546875" style="36" customWidth="1"/>
+    <col min="12" max="12" width="31.28515625" style="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -18101,20 +18180,20 @@
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.23046875" style="14"/>
-    <col min="3" max="3" width="28.23046875" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.23046875" style="14"/>
-    <col min="5" max="5" width="16.53515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.4609375" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.69140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.15234375" style="14" customWidth="1"/>
-    <col min="9" max="9" width="30.53515625" customWidth="1"/>
-    <col min="10" max="10" width="23.61328125" customWidth="1"/>
-    <col min="11" max="11" width="35.3046875" customWidth="1"/>
-    <col min="12" max="12" width="18.15234375" customWidth="1"/>
-    <col min="13" max="13" width="29.921875" customWidth="1"/>
+    <col min="1" max="2" width="9.28515625" style="14"/>
+    <col min="3" max="3" width="28.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="14"/>
+    <col min="5" max="5" width="16.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" style="14" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" customWidth="1"/>
+    <col min="11" max="11" width="35.28515625" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="13" max="13" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -23533,10 +23612,10 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.23046875" style="8"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -23571,7 +23650,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.9">
+    <row r="5" spans="1:2" ht="15.75">
       <c r="A5" t="s">
         <v>463</v>
       </c>
@@ -23579,7 +23658,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.9">
+    <row r="6" spans="1:2" ht="15.75">
       <c r="A6" t="s">
         <v>551</v>
       </c>
@@ -23587,7 +23666,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.9">
+    <row r="7" spans="1:2" ht="15.75">
       <c r="A7" t="s">
         <v>465</v>
       </c>
@@ -23595,7 +23674,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.9">
+    <row r="8" spans="1:2" ht="15.75">
       <c r="A8" t="s">
         <v>466</v>
       </c>
@@ -23603,7 +23682,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.9">
+    <row r="9" spans="1:2" ht="15.75">
       <c r="A9" t="s">
         <v>420</v>
       </c>
@@ -23611,7 +23690,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.9">
+    <row r="10" spans="1:2" ht="15.75">
       <c r="A10" t="s">
         <v>467</v>
       </c>
@@ -23619,7 +23698,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.9">
+    <row r="11" spans="1:2" ht="15.75">
       <c r="A11" t="s">
         <v>552</v>
       </c>
@@ -23627,7 +23706,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.9">
+    <row r="12" spans="1:2" ht="15.75">
       <c r="A12" t="s">
         <v>469</v>
       </c>
@@ -23635,7 +23714,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.9">
+    <row r="13" spans="1:2" ht="15.75">
       <c r="A13" t="s">
         <v>215</v>
       </c>
@@ -23643,7 +23722,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.9">
+    <row r="14" spans="1:2" ht="15.75">
       <c r="A14" t="s">
         <v>471</v>
       </c>
@@ -23651,7 +23730,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.9">
+    <row r="15" spans="1:2" ht="15.75">
       <c r="A15" t="s">
         <v>553</v>
       </c>
@@ -23659,7 +23738,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.9">
+    <row r="16" spans="1:2" ht="15.75">
       <c r="A16" t="s">
         <v>447</v>
       </c>
@@ -23667,7 +23746,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.9">
+    <row r="17" spans="1:2" ht="15.75">
       <c r="A17" t="s">
         <v>472</v>
       </c>
@@ -23675,7 +23754,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.9">
+    <row r="18" spans="1:2" ht="15.75">
       <c r="A18" t="s">
         <v>473</v>
       </c>
@@ -23683,7 +23762,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.9">
+    <row r="19" spans="1:2" ht="15.75">
       <c r="A19" t="s">
         <v>549</v>
       </c>
@@ -23691,7 +23770,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.9">
+    <row r="20" spans="1:2" ht="15.75">
       <c r="A20" t="s">
         <v>464</v>
       </c>
@@ -23699,7 +23778,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.9">
+    <row r="21" spans="1:2" ht="15.75">
       <c r="A21" t="s">
         <v>470</v>
       </c>
@@ -23707,7 +23786,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.9">
+    <row r="22" spans="1:2" ht="15.75">
       <c r="A22" t="s">
         <v>571</v>
       </c>
@@ -23726,28 +23805,28 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="H15" sqref="H15:H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.23046875" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="5" max="5" width="16.3046875" customWidth="1"/>
-    <col min="6" max="6" width="28.921875" customWidth="1"/>
-    <col min="7" max="7" width="19.765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.921875" style="14" customWidth="1"/>
-    <col min="9" max="9" width="19.765625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" style="14" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="67" t="s">
         <v>322</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="18" t="s">
@@ -24358,7 +24437,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="24.9">
+    <row r="23" spans="1:9" ht="25.5">
       <c r="A23" s="23" t="s">
         <v>300</v>
       </c>
@@ -24400,86 +24479,86 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="H19" sqref="H19:K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.3828125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="29.3828125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="25.765625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.07421875" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.3046875" style="14" customWidth="1"/>
-    <col min="8" max="8" width="22.3046875" style="14" customWidth="1"/>
-    <col min="9" max="9" width="17.765625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.61328125" style="14" customWidth="1"/>
-    <col min="12" max="12" width="8.921875" style="14" customWidth="1"/>
-    <col min="13" max="13" width="12.53515625" style="14" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.3828125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="29.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="25.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="14" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.5703125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="14" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" style="14" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="34" style="14" customWidth="1"/>
-    <col min="16" max="16" width="16.84375" style="14" customWidth="1"/>
-    <col min="17" max="17" width="18.15234375" style="14" customWidth="1"/>
-    <col min="18" max="18" width="74.3828125" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" style="14" customWidth="1"/>
+    <col min="17" max="17" width="18.140625" style="14" customWidth="1"/>
+    <col min="18" max="18" width="74.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="43" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.23046875" style="14"/>
+    <col min="20" max="16384" width="9.28515625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="57" customFormat="1">
-      <c r="A1" s="57" t="s">
-        <v>665</v>
-      </c>
-      <c r="B1" s="57" t="s">
+    <row r="1" spans="1:20" s="53" customFormat="1">
+      <c r="A1" s="53" t="s">
+        <v>663</v>
+      </c>
+      <c r="B1" s="53" t="s">
         <v>603</v>
       </c>
-      <c r="C1" s="57" t="s">
-        <v>666</v>
-      </c>
-      <c r="D1" s="57" t="s">
+      <c r="C1" s="53" t="s">
+        <v>664</v>
+      </c>
+      <c r="D1" s="53" t="s">
         <v>602</v>
       </c>
-      <c r="E1" s="57" t="s">
-        <v>662</v>
-      </c>
-      <c r="F1" s="57" t="s">
+      <c r="E1" s="53" t="s">
+        <v>660</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>667</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>668</v>
+      </c>
+      <c r="H1" s="53" t="s">
         <v>669</v>
       </c>
-      <c r="G1" s="57" t="s">
-        <v>670</v>
-      </c>
-      <c r="H1" s="57" t="s">
-        <v>671</v>
-      </c>
-      <c r="I1" s="57" t="s">
-        <v>659</v>
-      </c>
-      <c r="J1" s="57" t="s">
-        <v>625</v>
-      </c>
-      <c r="K1" s="57" t="s">
-        <v>637</v>
-      </c>
-      <c r="L1" s="57" t="s">
+      <c r="I1" s="53" t="s">
+        <v>657</v>
+      </c>
+      <c r="J1" s="53" t="s">
+        <v>623</v>
+      </c>
+      <c r="K1" s="53" t="s">
+        <v>635</v>
+      </c>
+      <c r="L1" s="53" t="s">
         <v>582</v>
       </c>
-      <c r="M1" s="57" t="s">
+      <c r="M1" s="53" t="s">
         <v>574</v>
       </c>
-      <c r="N1" s="57" t="s">
+      <c r="N1" s="53" t="s">
         <v>325</v>
       </c>
-      <c r="O1" s="57" t="s">
+      <c r="O1" s="53" t="s">
         <v>597</v>
       </c>
-      <c r="P1" s="57" t="s">
+      <c r="P1" s="53" t="s">
         <v>592</v>
       </c>
-      <c r="Q1" s="57" t="s">
-        <v>660</v>
-      </c>
-      <c r="R1" s="57" t="s">
+      <c r="Q1" s="53" t="s">
+        <v>658</v>
+      </c>
+      <c r="R1" s="53" t="s">
         <v>595</v>
       </c>
-      <c r="S1" s="57" t="s">
+      <c r="S1" s="53" t="s">
         <v>593</v>
       </c>
     </row>
@@ -24505,25 +24584,25 @@
       <c r="G2" s="14">
         <v>1</v>
       </c>
-      <c r="H2" s="55">
+      <c r="H2" s="51">
         <v>50</v>
       </c>
-      <c r="I2" s="55">
+      <c r="I2" s="51">
         <v>50</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="K2" s="14">
         <v>50</v>
       </c>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52">
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48">
         <v>50</v>
       </c>
-      <c r="O2" s="67" t="s">
-        <v>634</v>
+      <c r="O2" s="63" t="s">
+        <v>632</v>
       </c>
       <c r="S2" s="33"/>
       <c r="T2" s="33"/>
@@ -24532,10 +24611,10 @@
       <c r="A3" s="14" t="s">
         <v>573</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="47" t="s">
         <v>576</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="47" t="s">
         <v>576</v>
       </c>
       <c r="D3" s="14" t="s">
@@ -24550,38 +24629,38 @@
       <c r="G3" s="14">
         <v>1</v>
       </c>
-      <c r="H3" s="58" t="s">
+      <c r="H3" s="54" t="s">
+        <v>615</v>
+      </c>
+      <c r="I3" s="54" t="s">
+        <v>630</v>
+      </c>
+      <c r="J3" s="36" t="s">
         <v>616</v>
       </c>
-      <c r="I3" s="58" t="s">
-        <v>632</v>
-      </c>
-      <c r="J3" s="36" t="s">
-        <v>617</v>
-      </c>
-      <c r="K3" s="62">
+      <c r="K3" s="58">
         <f>I3*P3</f>
         <v>20.25</v>
       </c>
-      <c r="L3" s="65"/>
-      <c r="M3" s="52" t="s">
+      <c r="L3" s="61"/>
+      <c r="M3" s="48" t="s">
         <v>575</v>
       </c>
-      <c r="N3" s="66">
+      <c r="N3" s="62">
         <f>I3*P3</f>
         <v>20.25</v>
       </c>
       <c r="O3" s="33" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="P3" s="33">
         <v>13.5</v>
       </c>
       <c r="Q3" s="14" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="R3" s="14" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="S3" s="33"/>
       <c r="T3" s="33"/>
@@ -24590,10 +24669,10 @@
       <c r="A4" s="14" t="s">
         <v>573</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="47" t="s">
         <v>577</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="47" t="s">
         <v>577</v>
       </c>
       <c r="D4" s="14" t="s">
@@ -24608,27 +24687,27 @@
       <c r="G4" s="33">
         <v>1</v>
       </c>
-      <c r="H4" s="60">
+      <c r="H4" s="56">
         <v>22.5</v>
       </c>
-      <c r="I4" s="60">
+      <c r="I4" s="56">
         <v>22.5</v>
       </c>
       <c r="J4" s="33" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="K4" s="33">
         <v>22.5</v>
       </c>
-      <c r="L4" s="65"/>
-      <c r="M4" s="52" t="s">
+      <c r="L4" s="61"/>
+      <c r="M4" s="48" t="s">
         <v>578</v>
       </c>
-      <c r="N4" s="52">
+      <c r="N4" s="48">
         <v>22.5</v>
       </c>
       <c r="O4" s="33" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -24647,31 +24726,31 @@
       <c r="E5" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="51" t="s">
         <v>613</v>
       </c>
-      <c r="G5" s="53">
+      <c r="G5" s="49">
         <f>2/7</f>
         <v>0.2857142857142857</v>
       </c>
-      <c r="H5" s="60">
+      <c r="H5" s="56">
         <v>150</v>
       </c>
-      <c r="I5" s="60">
+      <c r="I5" s="56">
         <v>150</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="K5" s="36">
         <f>H5</f>
         <v>150</v>
       </c>
-      <c r="L5" s="52">
+      <c r="L5" s="48">
         <v>300</v>
       </c>
-      <c r="M5" s="52"/>
-      <c r="N5" s="54">
+      <c r="M5" s="48"/>
+      <c r="N5" s="50">
         <f>G5*K5</f>
         <v>42.857142857142854</v>
       </c>
@@ -24695,36 +24774,36 @@
       <c r="E6" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="51" t="s">
         <v>614</v>
       </c>
-      <c r="G6" s="53">
+      <c r="G6" s="49">
         <f>3/7</f>
         <v>0.42857142857142855</v>
       </c>
-      <c r="H6" s="60">
+      <c r="H6" s="56">
         <v>1</v>
       </c>
-      <c r="I6" s="60">
+      <c r="I6" s="56">
         <v>1</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="K6" s="36">
         <v>58</v>
       </c>
-      <c r="L6" s="52">
+      <c r="L6" s="48">
         <f>3*P6</f>
         <v>174</v>
       </c>
-      <c r="M6" s="52"/>
-      <c r="N6" s="54">
+      <c r="M6" s="48"/>
+      <c r="N6" s="50">
         <f>K6*G6</f>
         <v>24.857142857142854</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="P6" s="14">
         <v>58</v>
@@ -24755,37 +24834,37 @@
       <c r="E7" s="14" t="s">
         <v>607</v>
       </c>
-      <c r="F7" s="55" t="s">
+      <c r="F7" s="51" t="s">
         <v>614</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="49">
         <f>3/7</f>
         <v>0.42857142857142855</v>
       </c>
-      <c r="H7" s="55" t="s">
-        <v>615</v>
-      </c>
-      <c r="I7" s="55">
-        <v>375</v>
+      <c r="H7" s="51">
+        <v>150</v>
+      </c>
+      <c r="I7" s="51">
+        <v>150</v>
       </c>
       <c r="J7" s="36" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="K7" s="36">
         <f>I7</f>
-        <v>375</v>
-      </c>
-      <c r="L7" s="52">
+        <v>150</v>
+      </c>
+      <c r="L7" s="48">
         <f>I7*3</f>
-        <v>1125</v>
-      </c>
-      <c r="M7" s="52"/>
-      <c r="N7" s="54">
+        <v>450</v>
+      </c>
+      <c r="M7" s="48"/>
+      <c r="N7" s="50">
         <f>K7*G7</f>
-        <v>160.71428571428569</v>
+        <v>64.285714285714278</v>
       </c>
       <c r="O7" s="33" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -24804,37 +24883,37 @@
       <c r="E8" s="14" t="s">
         <v>608</v>
       </c>
-      <c r="F8" s="60" t="s">
-        <v>639</v>
-      </c>
-      <c r="G8" s="63">
+      <c r="F8" s="56" t="s">
+        <v>637</v>
+      </c>
+      <c r="G8" s="59">
         <f>1/7</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="H8" s="64">
+      <c r="H8" s="60">
         <v>150</v>
       </c>
-      <c r="I8" s="64">
+      <c r="I8" s="60">
         <v>150</v>
       </c>
       <c r="J8" s="33" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="K8" s="36">
         <f>H8</f>
         <v>150</v>
       </c>
-      <c r="L8" s="52">
+      <c r="L8" s="48">
         <f>1*K8</f>
         <v>150</v>
       </c>
-      <c r="M8" s="52"/>
-      <c r="N8" s="54">
+      <c r="M8" s="48"/>
+      <c r="N8" s="50">
         <f>G8*K8</f>
         <v>21.428571428571427</v>
       </c>
       <c r="O8" s="33" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -24853,35 +24932,35 @@
       <c r="E9" s="14" t="s">
         <v>604</v>
       </c>
-      <c r="F9" s="55">
+      <c r="F9" s="51">
         <v>4</v>
       </c>
       <c r="G9" s="14">
         <v>4</v>
       </c>
-      <c r="H9" s="55">
+      <c r="H9" s="51">
         <v>200</v>
       </c>
-      <c r="I9" s="55">
+      <c r="I9" s="51">
         <v>200</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="K9" s="14">
         <f>I9*P9</f>
         <v>206</v>
       </c>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52" t="s">
+      <c r="L9" s="48"/>
+      <c r="M9" s="48" t="s">
         <v>587</v>
       </c>
-      <c r="N9" s="52">
+      <c r="N9" s="48">
         <f>K9*G9</f>
         <v>824</v>
       </c>
       <c r="O9" s="33" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="P9" s="14">
         <v>1.03</v>
@@ -24909,29 +24988,29 @@
       <c r="E10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="59">
+      <c r="F10" s="55">
         <v>4</v>
       </c>
-      <c r="G10" s="50">
+      <c r="G10" s="46">
         <v>4</v>
       </c>
-      <c r="H10" s="55" t="s">
-        <v>629</v>
-      </c>
-      <c r="I10" s="55">
+      <c r="H10" s="51" t="s">
+        <v>627</v>
+      </c>
+      <c r="I10" s="51">
         <v>55</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="K10" s="14">
         <f>I10</f>
         <v>55</v>
       </c>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="52" t="s">
-        <v>622</v>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48" t="s">
+        <v>620</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -24950,32 +25029,32 @@
       <c r="E11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="59">
+      <c r="F11" s="55">
         <v>4</v>
       </c>
-      <c r="G11" s="50">
+      <c r="G11" s="46">
         <v>4</v>
       </c>
-      <c r="H11" s="55" t="s">
-        <v>630</v>
-      </c>
-      <c r="I11" s="55">
+      <c r="H11" s="51" t="s">
+        <v>628</v>
+      </c>
+      <c r="I11" s="51">
         <v>225</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="K11" s="14">
         <f t="shared" ref="K11:K14" si="0">I11</f>
         <v>225</v>
       </c>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52" t="s">
-        <v>623</v>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48" t="s">
+        <v>621</v>
       </c>
       <c r="O11" s="33" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="P11" s="33"/>
       <c r="Q11" s="33"/>
@@ -24987,7 +25066,7 @@
         <v>588</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C12" s="36" t="s">
         <v>591</v>
@@ -24998,29 +25077,29 @@
       <c r="E12" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="F12" s="59">
+      <c r="F12" s="55">
         <v>3</v>
       </c>
-      <c r="G12" s="50">
+      <c r="G12" s="46">
         <v>3</v>
       </c>
-      <c r="H12" s="55" t="s">
-        <v>619</v>
-      </c>
-      <c r="I12" s="55">
+      <c r="H12" s="51" t="s">
+        <v>618</v>
+      </c>
+      <c r="I12" s="51">
         <v>150</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="K12" s="14">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52" t="s">
-        <v>624</v>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48" t="s">
+        <v>622</v>
       </c>
       <c r="P12" s="33"/>
       <c r="Q12" s="33"/>
@@ -25032,7 +25111,7 @@
         <v>588</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>590</v>
@@ -25041,32 +25120,32 @@
         <v>611</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>663</v>
-      </c>
-      <c r="F13" s="59">
+        <v>661</v>
+      </c>
+      <c r="F13" s="55">
         <v>3</v>
       </c>
-      <c r="G13" s="50">
+      <c r="G13" s="46">
         <v>3</v>
       </c>
-      <c r="H13" s="55" t="s">
-        <v>631</v>
-      </c>
-      <c r="I13" s="55">
+      <c r="H13" s="51" t="s">
+        <v>629</v>
+      </c>
+      <c r="I13" s="51">
         <f>(70+100)/2</f>
         <v>85</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="K13" s="14">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52" t="s">
-        <v>621</v>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48" t="s">
+        <v>619</v>
       </c>
       <c r="P13" s="33"/>
       <c r="Q13" s="33"/>
@@ -25089,34 +25168,34 @@
       <c r="E14" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="F14" s="55">
+      <c r="F14" s="51">
         <v>2</v>
       </c>
       <c r="G14" s="14">
         <v>2</v>
       </c>
-      <c r="H14" s="55" t="s">
-        <v>618</v>
-      </c>
-      <c r="I14" s="55">
+      <c r="H14" s="51" t="s">
+        <v>617</v>
+      </c>
+      <c r="I14" s="51">
         <f>(125+150)/2</f>
         <v>137.5</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="K14" s="14">
         <f t="shared" si="0"/>
         <v>137.5</v>
       </c>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52">
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48">
         <f>K14*F14</f>
         <v>275</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="P14" s="33"/>
       <c r="Q14" s="33"/>
@@ -25125,10 +25204,10 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="14" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>519</v>
@@ -25139,31 +25218,31 @@
       <c r="E15" s="14" t="s">
         <v>612</v>
       </c>
-      <c r="F15" s="69" t="s">
-        <v>620</v>
-      </c>
-      <c r="G15" s="70">
-        <v>4</v>
+      <c r="F15" s="65" t="s">
+        <v>359</v>
+      </c>
+      <c r="G15" s="66" t="s">
+        <v>359</v>
       </c>
       <c r="H15" s="33">
         <v>1</v>
       </c>
-      <c r="I15" s="64">
+      <c r="I15" s="60">
         <v>1</v>
       </c>
       <c r="J15" s="33" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="K15" s="33">
         <v>7</v>
       </c>
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52" t="s">
-        <v>649</v>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48" t="s">
+        <v>647</v>
       </c>
       <c r="O15" s="33" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="P15" s="33"/>
       <c r="Q15" s="33"/>
@@ -25172,45 +25251,45 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="14" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>606</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>664</v>
-      </c>
-      <c r="F16" s="69" t="s">
-        <v>620</v>
-      </c>
-      <c r="G16" s="70">
-        <v>4</v>
+        <v>662</v>
+      </c>
+      <c r="F16" s="65" t="s">
+        <v>359</v>
+      </c>
+      <c r="G16" s="66" t="s">
+        <v>359</v>
       </c>
       <c r="H16" s="33">
         <v>1</v>
       </c>
-      <c r="I16" s="64">
+      <c r="I16" s="60">
         <v>1</v>
       </c>
       <c r="J16" s="33" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="K16" s="33">
         <v>3</v>
       </c>
-      <c r="L16" s="52"/>
-      <c r="M16" s="52"/>
-      <c r="N16" s="52" t="s">
-        <v>650</v>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48" t="s">
+        <v>648</v>
       </c>
       <c r="O16" s="33" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="P16" s="33"/>
       <c r="Q16" s="33"/>
@@ -25225,19 +25304,19 @@
         <v>470</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>432</v>
+        <v>674</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>206</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="F17" s="70">
-        <v>1</v>
-      </c>
-      <c r="G17" s="70">
-        <v>1</v>
+        <v>675</v>
+      </c>
+      <c r="F17" s="65" t="s">
+        <v>359</v>
+      </c>
+      <c r="G17" s="66" t="s">
+        <v>359</v>
       </c>
       <c r="H17" s="33">
         <v>0.5</v>
@@ -25246,20 +25325,20 @@
         <v>500</v>
       </c>
       <c r="J17" s="33" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="K17" s="33">
         <f>I17*P17</f>
         <v>505</v>
       </c>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="52">
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48" t="e">
         <f>K17*G17</f>
-        <v>505</v>
+        <v>#VALUE!</v>
       </c>
       <c r="O17" s="33" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="P17" s="14">
         <v>1.01</v>
@@ -25287,11 +25366,11 @@
       <c r="E18" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="F18" s="70">
-        <v>1</v>
-      </c>
-      <c r="G18" s="70">
-        <v>1</v>
+      <c r="F18" s="65" t="s">
+        <v>359</v>
+      </c>
+      <c r="G18" s="66" t="s">
+        <v>359</v>
       </c>
       <c r="H18" s="33">
         <v>0.25</v>
@@ -25300,20 +25379,20 @@
         <v>250</v>
       </c>
       <c r="J18" s="33" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="K18" s="33">
         <f>I18*P18</f>
         <v>247.5</v>
       </c>
-      <c r="L18" s="52"/>
-      <c r="M18" s="52"/>
-      <c r="N18" s="52">
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="48" t="e">
         <f>K18*G17</f>
-        <v>247.5</v>
+        <v>#VALUE!</v>
       </c>
       <c r="O18" s="33" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="P18" s="14">
         <v>0.99</v>
@@ -25326,22 +25405,60 @@
       </c>
     </row>
     <row r="19" spans="1:18">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="33"/>
-      <c r="R19" s="33"/>
+      <c r="A19" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>672</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>673</v>
+      </c>
+      <c r="F19" s="65" t="s">
+        <v>359</v>
+      </c>
+      <c r="G19" s="66" t="s">
+        <v>359</v>
+      </c>
+      <c r="H19" s="71">
+        <f>0.06</f>
+        <v>0.06</v>
+      </c>
+      <c r="I19" s="71">
+        <f>H19*1000</f>
+        <v>60</v>
+      </c>
+      <c r="J19" s="33" t="s">
+        <v>626</v>
+      </c>
+      <c r="K19" s="33">
+        <f>I19*P19</f>
+        <v>57</v>
+      </c>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="48" t="e">
+        <f>K19*G18</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O19" s="33" t="s">
+        <v>642</v>
+      </c>
+      <c r="P19" s="14">
+        <v>0.95</v>
+      </c>
+      <c r="Q19" s="14" t="s">
+        <v>594</v>
+      </c>
+      <c r="R19" s="14" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="33"/>
@@ -25349,10 +25466,10 @@
       <c r="C20" s="33"/>
     </row>
     <row r="21" spans="1:18">
-      <c r="A21" s="56"/>
-      <c r="B21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
+      <c r="A21" s="52"/>
+      <c r="B21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25362,29 +25479,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D393925C-EE04-49D3-96F8-D624C850C48D}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.3828125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.765625" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.3046875" style="14" customWidth="1"/>
-    <col min="4" max="16384" width="9.23046875" style="14"/>
+    <col min="1" max="1" width="29.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="14" customWidth="1"/>
+    <col min="4" max="16384" width="9.28515625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="57" customFormat="1">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:3" s="53" customFormat="1">
+      <c r="A1" s="53" t="s">
         <v>603</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="53" t="s">
         <v>602</v>
       </c>
-      <c r="C1" s="57" t="s">
-        <v>638</v>
+      <c r="C1" s="53" t="s">
+        <v>636</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -25399,7 +25516,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="47" t="s">
         <v>576</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -25410,7 +25527,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="47" t="s">
         <v>577</v>
       </c>
       <c r="B4" s="14" t="s">
@@ -25427,7 +25544,7 @@
       <c r="B5" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="C5" s="53">
+      <c r="C5" s="49">
         <f>2/7</f>
         <v>0.2857142857142857</v>
       </c>
@@ -25439,7 +25556,7 @@
       <c r="B6" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="C6" s="53">
+      <c r="C6" s="49">
         <f>3/7</f>
         <v>0.42857142857142855</v>
       </c>
@@ -25451,7 +25568,7 @@
       <c r="B7" s="14" t="s">
         <v>607</v>
       </c>
-      <c r="C7" s="53">
+      <c r="C7" s="49">
         <f>3/7</f>
         <v>0.42857142857142855</v>
       </c>
@@ -25463,7 +25580,7 @@
       <c r="B8" s="14" t="s">
         <v>608</v>
       </c>
-      <c r="C8" s="63">
+      <c r="C8" s="59">
         <f>1/7</f>
         <v>0.14285714285714285</v>
       </c>
@@ -25486,18 +25603,18 @@
       <c r="B10" s="14" t="s">
         <v>605</v>
       </c>
-      <c r="C10" s="50">
+      <c r="C10" s="46">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="14" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>611</v>
       </c>
-      <c r="C11" s="50">
+      <c r="C11" s="46">
         <v>3</v>
       </c>
     </row>
@@ -25514,13 +25631,13 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="14" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>606</v>
       </c>
-      <c r="C13" s="70">
-        <v>4</v>
+      <c r="C13" s="66" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -25530,16 +25647,16 @@
       <c r="B14" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="C14" s="70">
-        <v>1</v>
+      <c r="C14" s="66" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="C15" s="33"/>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="56"/>
-      <c r="B17" s="56"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25551,50 +25668,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767F6C5C-EB59-4436-B536-E20742AF84D3}">
   <dimension ref="A1:L123"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="29.3828125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="25.765625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.3046875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="17.765625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.61328125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="16.84375" style="14" customWidth="1"/>
-    <col min="10" max="10" width="18.15234375" style="14" customWidth="1"/>
-    <col min="11" max="16384" width="9.23046875" style="14"/>
+    <col min="1" max="2" width="29.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.5703125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="14" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" style="14" customWidth="1"/>
+    <col min="11" max="16384" width="9.28515625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="57" customFormat="1">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:12" s="53" customFormat="1">
+      <c r="A1" s="53" t="s">
         <v>603</v>
       </c>
-      <c r="B1" s="57" t="s">
-        <v>666</v>
-      </c>
-      <c r="C1" s="57" t="s">
+      <c r="B1" s="53" t="s">
+        <v>664</v>
+      </c>
+      <c r="C1" s="53" t="s">
         <v>602</v>
       </c>
-      <c r="D1" s="57" t="s">
-        <v>662</v>
-      </c>
-      <c r="E1" s="57" t="s">
-        <v>671</v>
-      </c>
-      <c r="F1" s="57" t="s">
-        <v>659</v>
-      </c>
-      <c r="G1" s="57" t="s">
-        <v>625</v>
-      </c>
-      <c r="H1" s="57" t="s">
-        <v>637</v>
-      </c>
-      <c r="I1" s="57" t="s">
+      <c r="D1" s="53" t="s">
+        <v>660</v>
+      </c>
+      <c r="E1" s="53" t="s">
+        <v>669</v>
+      </c>
+      <c r="F1" s="53" t="s">
+        <v>657</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>623</v>
+      </c>
+      <c r="H1" s="53" t="s">
+        <v>635</v>
+      </c>
+      <c r="I1" s="53" t="s">
         <v>592</v>
       </c>
-      <c r="J1" s="57" t="s">
-        <v>660</v>
+      <c r="J1" s="53" t="s">
+        <v>658</v>
       </c>
       <c r="L1" s="33"/>
     </row>
@@ -25611,14 +25730,14 @@
       <c r="D2" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="E2" s="55">
+      <c r="E2" s="51">
         <v>50</v>
       </c>
-      <c r="F2" s="55">
+      <c r="F2" s="51">
         <v>50</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H2" s="14">
         <v>50</v>
@@ -25627,10 +25746,10 @@
       <c r="L2" s="33"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="47" t="s">
         <v>576</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="47" t="s">
         <v>576</v>
       </c>
       <c r="C3" s="14" t="s">
@@ -25639,16 +25758,16 @@
       <c r="D3" s="14" t="s">
         <v>609</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="54" t="s">
+        <v>615</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>630</v>
+      </c>
+      <c r="G3" s="36" t="s">
         <v>616</v>
       </c>
-      <c r="F3" s="58" t="s">
-        <v>632</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>617</v>
-      </c>
-      <c r="H3" s="62">
+      <c r="H3" s="58">
         <f>F3*I3</f>
         <v>20.25</v>
       </c>
@@ -25656,16 +25775,16 @@
         <v>13.5</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="K3" s="33"/>
       <c r="L3" s="36"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="47" t="s">
         <v>577</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="47" t="s">
         <v>577</v>
       </c>
       <c r="C4" s="14" t="s">
@@ -25674,14 +25793,14 @@
       <c r="D4" s="14" t="s">
         <v>610</v>
       </c>
-      <c r="E4" s="60">
+      <c r="E4" s="56">
         <v>22.5</v>
       </c>
-      <c r="F4" s="60">
+      <c r="F4" s="56">
         <v>22.5</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H4" s="33">
         <v>22.5</v>
@@ -25701,14 +25820,14 @@
       <c r="D5" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="E5" s="60">
+      <c r="E5" s="56">
         <v>150</v>
       </c>
-      <c r="F5" s="60">
+      <c r="F5" s="56">
         <v>150</v>
       </c>
       <c r="G5" s="36" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H5" s="36">
         <f>E5</f>
@@ -25729,14 +25848,14 @@
       <c r="D6" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="E6" s="60">
+      <c r="E6" s="56">
         <v>1</v>
       </c>
-      <c r="F6" s="60">
+      <c r="F6" s="56">
         <v>1</v>
       </c>
       <c r="G6" s="36" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="H6" s="36">
         <v>58</v>
@@ -25762,18 +25881,18 @@
       <c r="D7" s="14" t="s">
         <v>607</v>
       </c>
-      <c r="E7" s="55" t="s">
-        <v>615</v>
-      </c>
-      <c r="F7" s="55">
-        <v>375</v>
+      <c r="E7" s="51">
+        <v>150</v>
+      </c>
+      <c r="F7" s="51">
+        <v>150</v>
       </c>
       <c r="G7" s="36" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H7" s="36">
         <f>F7</f>
-        <v>375</v>
+        <v>150</v>
       </c>
       <c r="L7" s="33"/>
     </row>
@@ -25790,14 +25909,14 @@
       <c r="D8" s="14" t="s">
         <v>608</v>
       </c>
-      <c r="E8" s="64">
+      <c r="E8" s="60">
         <v>150</v>
       </c>
-      <c r="F8" s="64">
+      <c r="F8" s="60">
         <v>150</v>
       </c>
       <c r="G8" s="33" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H8" s="36">
         <f>E8</f>
@@ -25818,14 +25937,14 @@
       <c r="D9" s="14" t="s">
         <v>604</v>
       </c>
-      <c r="E9" s="55">
+      <c r="E9" s="51">
         <v>200</v>
       </c>
-      <c r="F9" s="55">
+      <c r="F9" s="51">
         <v>200</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="H9" s="14">
         <f>F9*I9</f>
@@ -25852,14 +25971,14 @@
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="55" t="s">
-        <v>629</v>
-      </c>
-      <c r="F10" s="55">
+      <c r="E10" s="51" t="s">
+        <v>627</v>
+      </c>
+      <c r="F10" s="51">
         <v>55</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H10" s="14">
         <f>F10</f>
@@ -25880,14 +25999,14 @@
       <c r="D11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="55" t="s">
-        <v>630</v>
-      </c>
-      <c r="F11" s="55">
+      <c r="E11" s="51" t="s">
+        <v>628</v>
+      </c>
+      <c r="F11" s="51">
         <v>225</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H11" s="14">
         <f t="shared" ref="H11:H14" si="0">F11</f>
@@ -25899,7 +26018,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="14" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B12" s="36" t="s">
         <v>591</v>
@@ -25910,14 +26029,14 @@
       <c r="D12" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="E12" s="55" t="s">
-        <v>619</v>
-      </c>
-      <c r="F12" s="55">
+      <c r="E12" s="51" t="s">
+        <v>618</v>
+      </c>
+      <c r="F12" s="51">
         <v>150</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H12" s="14">
         <f t="shared" si="0"/>
@@ -25929,7 +26048,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="14" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>590</v>
@@ -25938,17 +26057,17 @@
         <v>611</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>663</v>
-      </c>
-      <c r="E13" s="55" t="s">
-        <v>631</v>
-      </c>
-      <c r="F13" s="55">
+        <v>661</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>629</v>
+      </c>
+      <c r="F13" s="51">
         <f>(70+100)/2</f>
         <v>85</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H13" s="14">
         <f t="shared" si="0"/>
@@ -25971,15 +26090,15 @@
       <c r="D14" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="E14" s="55" t="s">
-        <v>618</v>
-      </c>
-      <c r="F14" s="55">
+      <c r="E14" s="51" t="s">
+        <v>617</v>
+      </c>
+      <c r="F14" s="51">
         <f>(125+150)/2</f>
         <v>137.5</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H14" s="14">
         <f t="shared" si="0"/>
@@ -25991,7 +26110,7 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="14" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>519</v>
@@ -26005,11 +26124,11 @@
       <c r="E15" s="33">
         <v>1</v>
       </c>
-      <c r="F15" s="64">
+      <c r="F15" s="60">
         <v>1</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="H15" s="33">
         <v>7</v>
@@ -26020,25 +26139,25 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="14" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>606</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="E16" s="33">
         <v>1</v>
       </c>
-      <c r="F16" s="64">
+      <c r="F16" s="60">
         <v>1</v>
       </c>
       <c r="G16" s="33" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="H16" s="33">
         <v>3</v>
@@ -26052,13 +26171,13 @@
         <v>470</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>432</v>
+        <v>674</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>206</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>208</v>
+        <v>675</v>
       </c>
       <c r="E17" s="33">
         <v>0.5</v>
@@ -26067,7 +26186,7 @@
         <v>500</v>
       </c>
       <c r="G17" s="33" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="H17" s="33">
         <f>F17*I17</f>
@@ -26101,7 +26220,7 @@
         <v>250</v>
       </c>
       <c r="G18" s="33" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="H18" s="33">
         <f>F18*I18</f>
@@ -26116,22 +26235,45 @@
       <c r="L18" s="36"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="B19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
+      <c r="A19" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>672</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>673</v>
+      </c>
+      <c r="E19" s="71">
+        <v>0.06</v>
+      </c>
+      <c r="F19" s="72">
+        <v>60</v>
+      </c>
+      <c r="G19" s="33" t="s">
+        <v>626</v>
+      </c>
+      <c r="H19" s="59">
+        <v>57</v>
+      </c>
+      <c r="I19" s="14">
+        <v>0.95</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>594</v>
+      </c>
       <c r="L19"/>
     </row>
     <row r="20" spans="1:12">
       <c r="L20"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
+      <c r="A21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
       <c r="L21"/>
     </row>
     <row r="22" spans="1:12">
@@ -26454,15 +26596,15 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.69140625" customWidth="1"/>
-    <col min="2" max="2" width="18.61328125" customWidth="1"/>
-    <col min="3" max="3" width="24.61328125" customWidth="1"/>
-    <col min="4" max="4" width="14.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="20.921875" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="14" customFormat="1">
@@ -27232,16 +27374,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF17F7E9-319B-4EE9-87FA-1B8B59FCFD55}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E122" sqref="E122"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="E124" sqref="E124:F124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.23046875" customWidth="1"/>
-    <col min="3" max="3" width="27.4609375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.4609375" style="33" customWidth="1"/>
-    <col min="6" max="6" width="18.61328125" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" style="33" customWidth="1"/>
+    <col min="6" max="6" width="74.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -27258,10 +27400,10 @@
         <v>602</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="F1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -27282,7 +27424,7 @@
         <v>0.30699999999999994</v>
       </c>
       <c r="F2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -27524,7 +27666,7 @@
         <v>0.89769999999999994</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" s="14" t="s">
         <v>44</v>
       </c>
@@ -27542,7 +27684,7 @@
         <v>0.86980000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18" s="14" t="s">
         <v>46</v>
       </c>
@@ -27559,7 +27701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19" s="14" t="s">
         <v>49</v>
       </c>
@@ -27576,7 +27718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20" s="14" t="s">
         <v>51</v>
       </c>
@@ -27593,7 +27735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" s="14" t="s">
         <v>53</v>
       </c>
@@ -27610,10 +27752,10 @@
         <v>0.5</v>
       </c>
       <c r="F21" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="14" t="s">
         <v>55</v>
       </c>
@@ -27630,7 +27772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" s="14" t="s">
         <v>58</v>
       </c>
@@ -27647,10 +27789,10 @@
         <v>0.3</v>
       </c>
       <c r="F23" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="14" t="s">
         <v>60</v>
       </c>
@@ -27667,7 +27809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="A25" s="14" t="s">
         <v>62</v>
       </c>
@@ -27684,7 +27826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="A26" s="14" t="s">
         <v>64</v>
       </c>
@@ -27699,7 +27841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27" s="14" t="s">
         <v>66</v>
       </c>
@@ -27716,7 +27858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28" s="14" t="s">
         <v>68</v>
       </c>
@@ -27733,7 +27875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="A29" s="14" t="s">
         <v>70</v>
       </c>
@@ -27748,7 +27890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7">
       <c r="A30" s="14" t="s">
         <v>72</v>
       </c>
@@ -27765,7 +27907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:7">
       <c r="A31" s="14" t="s">
         <v>74</v>
       </c>
@@ -27782,7 +27924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:7">
       <c r="A32" s="14" t="s">
         <v>76</v>
       </c>
@@ -27796,10 +27938,16 @@
         <v>611</v>
       </c>
       <c r="E32" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G32" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="14" t="s">
         <v>78</v>
       </c>
@@ -27813,10 +27961,16 @@
         <v>611</v>
       </c>
       <c r="E33" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="14" t="s">
         <v>80</v>
       </c>
@@ -27830,10 +27984,16 @@
         <v>611</v>
       </c>
       <c r="E34" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="14" t="s">
         <v>82</v>
       </c>
@@ -27847,10 +28007,13 @@
         <v>295</v>
       </c>
       <c r="E35" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="14" t="s">
         <v>84</v>
       </c>
@@ -27864,10 +28027,13 @@
         <v>295</v>
       </c>
       <c r="E36" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="14" t="s">
         <v>86</v>
       </c>
@@ -27881,10 +28047,13 @@
         <v>295</v>
       </c>
       <c r="E37" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="14" t="s">
         <v>88</v>
       </c>
@@ -27898,10 +28067,13 @@
         <v>295</v>
       </c>
       <c r="E38" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="14" t="s">
         <v>90</v>
       </c>
@@ -27915,10 +28087,13 @@
         <v>295</v>
       </c>
       <c r="E39" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="14" t="s">
         <v>92</v>
       </c>
@@ -27932,10 +28107,13 @@
         <v>295</v>
       </c>
       <c r="E40" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="14" t="s">
         <v>94</v>
       </c>
@@ -27949,10 +28127,13 @@
         <v>295</v>
       </c>
       <c r="E41" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="14" t="s">
         <v>96</v>
       </c>
@@ -27966,10 +28147,13 @@
         <v>295</v>
       </c>
       <c r="E42" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="14" t="s">
         <v>98</v>
       </c>
@@ -27983,10 +28167,13 @@
         <v>295</v>
       </c>
       <c r="E43" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="14" t="s">
         <v>100</v>
       </c>
@@ -28000,10 +28187,13 @@
         <v>295</v>
       </c>
       <c r="E44" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="14" t="s">
         <v>102</v>
       </c>
@@ -28017,10 +28207,13 @@
         <v>295</v>
       </c>
       <c r="E45" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>0.27</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="14" t="s">
         <v>104</v>
       </c>
@@ -28037,10 +28230,10 @@
         <v>0.3</v>
       </c>
       <c r="F46" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="14" t="s">
         <v>107</v>
       </c>
@@ -28057,10 +28250,10 @@
         <v>0.2</v>
       </c>
       <c r="F47" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="14" t="s">
         <v>109</v>
       </c>
@@ -29127,9 +29320,9 @@
         <v>0.34</v>
       </c>
       <c r="F114" t="s">
-        <v>657</v>
-      </c>
-      <c r="G114" s="56"/>
+        <v>655</v>
+      </c>
+      <c r="G114" s="52"/>
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="14" t="s">
@@ -29148,7 +29341,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="F115" s="14" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -29168,7 +29361,7 @@
         <v>0.29499999999999998</v>
       </c>
       <c r="F116" s="14" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -29188,7 +29381,7 @@
         <v>0.40500000000000003</v>
       </c>
       <c r="F117" s="14" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -29208,7 +29401,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="F118" s="14" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -29228,7 +29421,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="F119" s="14" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -29309,7 +29502,10 @@
         <v>283</v>
       </c>
       <c r="E124" s="14">
-        <v>0</v>
+        <v>0.45</v>
+      </c>
+      <c r="F124" t="s">
+        <v>671</v>
       </c>
     </row>
   </sheetData>
@@ -29325,20 +29521,20 @@
       <selection activeCell="D64" sqref="D64:F64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.23046875" style="14"/>
-    <col min="3" max="3" width="28.23046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.28515625" style="14"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="68" t="s">
         <v>373</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="49"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="E1" s="69"/>
+      <c r="F1" s="70"/>
+    </row>
+    <row r="2" spans="1:6" ht="30">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -31717,19 +31913,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J94" sqref="J94"/>
+    <sheetView topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="28.23046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.53515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.4609375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.15234375" customWidth="1"/>
-    <col min="9" max="10" width="30.15234375" style="14" customWidth="1"/>
-    <col min="11" max="11" width="16.15234375" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" customWidth="1"/>
+    <col min="9" max="10" width="30.140625" style="14" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -31761,7 +31957,7 @@
         <v>602</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="K1" s="14" t="s">
         <v>365</v>
@@ -34937,7 +35133,7 @@
       </c>
       <c r="J93" s="14" t="str">
         <f>VLOOKUP(B93,concordance!$B$2:$Q$124,15,FALSE)</f>
-        <v>Beer</v>
+        <v>Beer and cider</v>
       </c>
       <c r="K93" s="14" t="s">
         <v>206</v>
@@ -34970,11 +35166,11 @@
       </c>
       <c r="I94" s="14" t="str">
         <f>VLOOKUP(B94,concordance!$B$2:$Q$124,14,FALSE)</f>
-        <v>Others</v>
+        <v>Alcohol</v>
       </c>
       <c r="J94" s="14" t="str">
         <f>VLOOKUP(B94,concordance!$B$2:$Q$124,15,FALSE)</f>
-        <v>Others</v>
+        <v>Beer and cider</v>
       </c>
       <c r="K94" s="14" t="s">
         <v>206</v>
@@ -35007,11 +35203,11 @@
       </c>
       <c r="I95" s="14" t="str">
         <f>VLOOKUP(B95,concordance!$B$2:$Q$124,14,FALSE)</f>
-        <v>Others</v>
+        <v>Alcohol</v>
       </c>
       <c r="J95" s="14" t="str">
         <f>VLOOKUP(B95,concordance!$B$2:$Q$124,15,FALSE)</f>
-        <v>Others</v>
+        <v>Spirits</v>
       </c>
       <c r="K95" s="14" t="s">
         <v>206</v>

</xml_diff>

<commit_message>
change meat in EP 2.0, adapt losses and waste groups
</commit_message>
<xml_diff>
--- a/inst/items_conc.xlsx
+++ b/inst/items_conc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="concordance" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6517" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6492" uniqueCount="705">
   <si>
     <t>comm_code</t>
   </si>
@@ -1935,9 +1935,6 @@
     <t>70 - 100</t>
   </si>
   <si>
-    <t>1.5</t>
-  </si>
-  <si>
     <t>assuming  3 Portions</t>
   </si>
   <si>
@@ -1959,12 +1956,6 @@
     <t>&lt;=1/week</t>
   </si>
   <si>
-    <t>all other meat types</t>
-  </si>
-  <si>
-    <t>only include poultry here</t>
-  </si>
-  <si>
     <t>assuming 7g per cup</t>
   </si>
   <si>
@@ -2127,18 +2118,6 @@
     <t>assumed 1 - average edible flesh share across all fish species</t>
   </si>
   <si>
-    <t>200-250</t>
-  </si>
-  <si>
-    <t>100-200</t>
-  </si>
-  <si>
-    <t>70-100</t>
-  </si>
-  <si>
-    <t>125-150</t>
-  </si>
-  <si>
     <t>eat_group_fin_2</t>
   </si>
   <si>
@@ -2170,6 +2149,18 @@
   </si>
   <si>
     <t>Dairy products</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>only include poultry here and assume 2 Portions of size 125 g</t>
+  </si>
+  <si>
+    <t>all other meat types, assuming 1 Potion of 125 g</t>
+  </si>
+  <si>
+    <t>100-150</t>
   </si>
 </sst>
 </file>
@@ -2857,7 +2848,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -2946,7 +2937,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="41" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2984,7 +2974,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3000,6 +2989,13 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="41" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="41" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -3359,11 +3355,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R18" sqref="R18:R28"/>
+      <selection pane="bottomRight" activeCell="R57" sqref="R57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3428,7 +3424,7 @@
         <v>370</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>321</v>
@@ -3437,7 +3433,7 @@
         <v>601</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="R1" s="14" t="s">
         <v>364</v>
@@ -4375,13 +4371,13 @@
         <v>299</v>
       </c>
       <c r="O18" s="24" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="P18" s="14" t="s">
         <v>610</v>
       </c>
       <c r="Q18" s="33" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="R18" s="14" t="s">
         <v>381</v>
@@ -4431,13 +4427,13 @@
         <v>299</v>
       </c>
       <c r="O19" s="24" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="P19" s="14" t="s">
         <v>610</v>
       </c>
       <c r="Q19" s="33" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="R19" s="14" t="s">
         <v>381</v>
@@ -4487,13 +4483,13 @@
         <v>299</v>
       </c>
       <c r="O20" s="24" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="P20" s="14" t="s">
         <v>610</v>
       </c>
       <c r="Q20" s="33" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="R20" s="14" t="s">
         <v>381</v>
@@ -4543,7 +4539,7 @@
         <v>299</v>
       </c>
       <c r="O21" s="24" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="P21" s="14" t="s">
         <v>608</v>
@@ -4599,13 +4595,13 @@
         <v>299</v>
       </c>
       <c r="O22" s="24" t="s">
-        <v>698</v>
+        <v>691</v>
       </c>
       <c r="P22" s="14" t="s">
         <v>610</v>
       </c>
       <c r="Q22" s="33" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="R22" s="14" t="s">
         <v>381</v>
@@ -4657,7 +4653,7 @@
       <c r="O23" s="24" t="s">
         <v>309</v>
       </c>
-      <c r="P23" s="57" t="s">
+      <c r="P23" s="56" t="s">
         <v>608</v>
       </c>
       <c r="Q23" s="33" t="s">
@@ -4711,7 +4707,7 @@
         <v>299</v>
       </c>
       <c r="O24" s="24" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="P24" s="14" t="s">
         <v>608</v>
@@ -4765,7 +4761,7 @@
         <v>299</v>
       </c>
       <c r="O25" s="34" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="P25" s="17" t="s">
         <v>608</v>
@@ -4863,7 +4859,7 @@
         <v>299</v>
       </c>
       <c r="O27" s="24" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="P27" s="17" t="s">
         <v>608</v>
@@ -4917,7 +4913,7 @@
         <v>299</v>
       </c>
       <c r="O28" s="24" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="P28" s="33" t="s">
         <v>608</v>
@@ -5069,13 +5065,13 @@
         <v>299</v>
       </c>
       <c r="O31" s="24" t="s">
-        <v>699</v>
-      </c>
-      <c r="P31" s="14" t="s">
-        <v>610</v>
-      </c>
-      <c r="Q31" s="33" t="s">
-        <v>288</v>
+        <v>692</v>
+      </c>
+      <c r="P31" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="Q31" s="17" t="s">
+        <v>608</v>
       </c>
       <c r="R31" s="14" t="s">
         <v>381</v>
@@ -5905,10 +5901,10 @@
       <c r="O46" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="P46" s="57" t="s">
-        <v>668</v>
-      </c>
-      <c r="Q46" s="57" t="s">
+      <c r="P46" s="56" t="s">
+        <v>665</v>
+      </c>
+      <c r="Q46" s="56" t="s">
         <v>611</v>
       </c>
       <c r="R46" s="14" t="s">
@@ -5955,11 +5951,11 @@
       <c r="O47" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="P47" s="57" t="s">
-        <v>668</v>
-      </c>
-      <c r="Q47" s="57" t="s">
-        <v>688</v>
+      <c r="P47" s="56" t="s">
+        <v>665</v>
+      </c>
+      <c r="Q47" s="56" t="s">
+        <v>685</v>
       </c>
       <c r="R47" s="14" t="s">
         <v>106</v>
@@ -6005,11 +6001,11 @@
       <c r="O48" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="P48" s="57" t="s">
-        <v>668</v>
-      </c>
-      <c r="Q48" s="57" t="s">
-        <v>659</v>
+      <c r="P48" s="56" t="s">
+        <v>665</v>
+      </c>
+      <c r="Q48" s="56" t="s">
+        <v>656</v>
       </c>
       <c r="R48" s="14" t="s">
         <v>106</v>
@@ -6048,16 +6044,16 @@
       </c>
       <c r="L49" s="9"/>
       <c r="M49" s="1"/>
-      <c r="N49" s="69" t="s">
+      <c r="N49" s="67" t="s">
         <v>300</v>
       </c>
-      <c r="O49" s="69" t="s">
+      <c r="O49" s="67" t="s">
         <v>300</v>
       </c>
-      <c r="P49" s="57" t="s">
+      <c r="P49" s="56" t="s">
         <v>383</v>
       </c>
-      <c r="Q49" s="57" t="s">
+      <c r="Q49" s="56" t="s">
         <v>383</v>
       </c>
       <c r="R49" s="14" t="s">
@@ -6104,16 +6100,16 @@
       <c r="M50" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="N50" s="69" t="s">
+      <c r="N50" s="67" t="s">
         <v>300</v>
       </c>
-      <c r="O50" s="69" t="s">
+      <c r="O50" s="67" t="s">
         <v>300</v>
       </c>
-      <c r="P50" s="57" t="s">
+      <c r="P50" s="56" t="s">
         <v>383</v>
       </c>
-      <c r="Q50" s="57" t="s">
+      <c r="Q50" s="56" t="s">
         <v>383</v>
       </c>
       <c r="R50" s="14" t="s">
@@ -6160,16 +6156,16 @@
       <c r="M51" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="N51" s="69" t="s">
+      <c r="N51" s="67" t="s">
         <v>300</v>
       </c>
-      <c r="O51" s="69" t="s">
+      <c r="O51" s="67" t="s">
         <v>300</v>
       </c>
-      <c r="P51" s="57" t="s">
+      <c r="P51" s="56" t="s">
         <v>383</v>
       </c>
-      <c r="Q51" s="57" t="s">
+      <c r="Q51" s="56" t="s">
         <v>383</v>
       </c>
       <c r="R51" s="14" t="s">
@@ -6216,16 +6212,16 @@
       <c r="M52" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="N52" s="69" t="s">
+      <c r="N52" s="67" t="s">
         <v>300</v>
       </c>
-      <c r="O52" s="69" t="s">
+      <c r="O52" s="67" t="s">
         <v>300</v>
       </c>
-      <c r="P52" s="57" t="s">
+      <c r="P52" s="56" t="s">
         <v>383</v>
       </c>
-      <c r="Q52" s="57" t="s">
+      <c r="Q52" s="56" t="s">
         <v>383</v>
       </c>
       <c r="R52" s="14" t="s">
@@ -6272,16 +6268,16 @@
       <c r="M53" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="N53" s="69" t="s">
+      <c r="N53" s="67" t="s">
         <v>300</v>
       </c>
-      <c r="O53" s="69" t="s">
+      <c r="O53" s="67" t="s">
         <v>300</v>
       </c>
-      <c r="P53" s="57" t="s">
+      <c r="P53" s="56" t="s">
         <v>383</v>
       </c>
-      <c r="Q53" s="57" t="s">
+      <c r="Q53" s="56" t="s">
         <v>383</v>
       </c>
       <c r="R53" s="14" t="s">
@@ -6703,7 +6699,7 @@
         <v>299</v>
       </c>
       <c r="O65" s="34" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="P65" s="17" t="s">
         <v>608</v>
@@ -7963,10 +7959,10 @@
       <c r="O91" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="P91" s="64" t="s">
+      <c r="P91" s="63" t="s">
         <v>206</v>
       </c>
-      <c r="Q91" s="64" t="s">
+      <c r="Q91" s="63" t="s">
         <v>205</v>
       </c>
       <c r="R91" s="14" t="s">
@@ -8019,11 +8015,11 @@
       <c r="O92" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="P92" s="64" t="s">
+      <c r="P92" s="63" t="s">
         <v>206</v>
       </c>
-      <c r="Q92" s="64" t="s">
-        <v>672</v>
+      <c r="Q92" s="63" t="s">
+        <v>669</v>
       </c>
       <c r="R92" s="14" t="s">
         <v>206</v>
@@ -8075,11 +8071,11 @@
       <c r="O93" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="P93" s="64" t="s">
+      <c r="P93" s="63" t="s">
         <v>206</v>
       </c>
-      <c r="Q93" s="64" t="s">
-        <v>672</v>
+      <c r="Q93" s="63" t="s">
+        <v>669</v>
       </c>
       <c r="R93" s="14" t="s">
         <v>206</v>
@@ -8131,11 +8127,11 @@
       <c r="O94" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="P94" s="64" t="s">
+      <c r="P94" s="63" t="s">
         <v>206</v>
       </c>
-      <c r="Q94" s="64" t="s">
-        <v>670</v>
+      <c r="Q94" s="63" t="s">
+        <v>667</v>
       </c>
       <c r="R94" s="14" t="s">
         <v>206</v>
@@ -9414,13 +9410,13 @@
         <v>601</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="G1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -9789,10 +9785,10 @@
         <v>0.5</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="G21" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -9988,10 +9984,10 @@
         <v>0.27</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -10012,10 +10008,10 @@
         <v>0.27</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -10036,10 +10032,10 @@
         <v>0.27</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -10060,7 +10056,7 @@
         <v>0.27</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G35" s="14"/>
     </row>
@@ -10082,7 +10078,7 @@
         <v>0.27</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G36" s="14"/>
     </row>
@@ -10104,7 +10100,7 @@
         <v>0.27</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G37" s="14"/>
     </row>
@@ -10126,7 +10122,7 @@
         <v>0.27</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G38" s="14"/>
     </row>
@@ -10148,7 +10144,7 @@
         <v>0.27</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G39" s="14"/>
     </row>
@@ -10170,7 +10166,7 @@
         <v>0.27</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G40" s="14"/>
     </row>
@@ -10192,7 +10188,7 @@
         <v>0.27</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G41" s="14"/>
     </row>
@@ -10214,7 +10210,7 @@
         <v>0.27</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G42" s="14"/>
     </row>
@@ -10236,7 +10232,7 @@
         <v>0.27</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G43" s="14"/>
     </row>
@@ -10258,7 +10254,7 @@
         <v>0.27</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G44" s="14"/>
     </row>
@@ -10280,7 +10276,7 @@
         <v>0.27</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G45" s="14"/>
     </row>
@@ -10302,7 +10298,7 @@
         <v>0.3</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -10323,7 +10319,7 @@
         <v>0.2</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -11439,7 +11435,7 @@
         <v>0.34</v>
       </c>
       <c r="F115" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -11459,7 +11455,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="F116" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -11479,7 +11475,7 @@
         <v>0.29499999999999998</v>
       </c>
       <c r="F117" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -11499,7 +11495,7 @@
         <v>0.40500000000000003</v>
       </c>
       <c r="F118" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -11519,7 +11515,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="F119" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -11539,7 +11535,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="F120" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -11592,7 +11588,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="F123" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -11645,11 +11641,11 @@
       <c r="E126" s="14">
         <v>0.45</v>
       </c>
-      <c r="F126" s="52" t="s">
-        <v>691</v>
+      <c r="F126" s="51" t="s">
+        <v>688</v>
       </c>
       <c r="G126" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
   </sheetData>
@@ -11676,11 +11672,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="70" t="s">
         <v>372</v>
       </c>
-      <c r="E1" s="73"/>
-      <c r="F1" s="74"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="72"/>
     </row>
     <row r="2" spans="1:6" ht="30">
       <c r="A2" s="14" t="s">
@@ -14214,8 +14210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N124"/>
   <sheetViews>
-    <sheetView topLeftCell="G4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView topLeftCell="G97" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G120" sqref="A120:XFD120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -14264,7 +14260,7 @@
         <v>485</v>
       </c>
       <c r="J1" s="33" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="K1" s="33" t="s">
         <v>486</v>
@@ -14276,7 +14272,7 @@
         <v>488</v>
       </c>
       <c r="N1" s="33" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -14931,7 +14927,7 @@
         <v>484</v>
       </c>
       <c r="N16" s="45" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -14970,7 +14966,7 @@
         <v>484</v>
       </c>
       <c r="N17" s="45" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -15004,8 +15000,8 @@
       <c r="J18" s="17" t="s">
         <v>549</v>
       </c>
-      <c r="K18" s="57" t="s">
-        <v>674</v>
+      <c r="K18" s="56" t="s">
+        <v>671</v>
       </c>
       <c r="L18" s="41" t="s">
         <v>480</v>
@@ -15013,8 +15009,8 @@
       <c r="M18" s="17" t="s">
         <v>553</v>
       </c>
-      <c r="N18" s="57" t="s">
-        <v>658</v>
+      <c r="N18" s="56" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -15048,8 +15044,8 @@
       <c r="J19" s="17" t="s">
         <v>549</v>
       </c>
-      <c r="K19" s="57" t="s">
-        <v>674</v>
+      <c r="K19" s="56" t="s">
+        <v>671</v>
       </c>
       <c r="L19" s="41" t="s">
         <v>480</v>
@@ -15057,8 +15053,8 @@
       <c r="M19" s="17" t="s">
         <v>553</v>
       </c>
-      <c r="N19" s="57" t="s">
-        <v>658</v>
+      <c r="N19" s="56" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -15092,8 +15088,8 @@
       <c r="J20" s="17" t="s">
         <v>549</v>
       </c>
-      <c r="K20" s="57" t="s">
-        <v>674</v>
+      <c r="K20" s="56" t="s">
+        <v>671</v>
       </c>
       <c r="L20" s="41" t="s">
         <v>480</v>
@@ -15101,8 +15097,8 @@
       <c r="M20" s="17" t="s">
         <v>553</v>
       </c>
-      <c r="N20" s="57" t="s">
-        <v>658</v>
+      <c r="N20" s="56" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -15136,8 +15132,8 @@
       <c r="J21" s="17" t="s">
         <v>549</v>
       </c>
-      <c r="K21" s="57" t="s">
-        <v>679</v>
+      <c r="K21" s="56" t="s">
+        <v>676</v>
       </c>
       <c r="L21" s="41" t="s">
         <v>480</v>
@@ -15145,8 +15141,8 @@
       <c r="M21" s="17" t="s">
         <v>553</v>
       </c>
-      <c r="N21" s="57" t="s">
-        <v>702</v>
+      <c r="N21" s="56" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -15180,8 +15176,8 @@
       <c r="J22" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="K22" s="57" t="s">
-        <v>674</v>
+      <c r="K22" s="56" t="s">
+        <v>671</v>
       </c>
       <c r="L22" s="41" t="s">
         <v>480</v>
@@ -15189,8 +15185,8 @@
       <c r="M22" s="17" t="s">
         <v>553</v>
       </c>
-      <c r="N22" s="57" t="s">
-        <v>658</v>
+      <c r="N22" s="56" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -15224,8 +15220,8 @@
       <c r="J23" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="K23" s="57" t="s">
-        <v>679</v>
+      <c r="K23" s="56" t="s">
+        <v>676</v>
       </c>
       <c r="L23" s="41" t="s">
         <v>480</v>
@@ -15233,8 +15229,8 @@
       <c r="M23" s="17" t="s">
         <v>553</v>
       </c>
-      <c r="N23" s="57" t="s">
-        <v>702</v>
+      <c r="N23" s="56" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -15268,8 +15264,8 @@
       <c r="J24" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="K24" s="57" t="s">
-        <v>679</v>
+      <c r="K24" s="56" t="s">
+        <v>676</v>
       </c>
       <c r="L24" s="41" t="s">
         <v>480</v>
@@ -15277,8 +15273,8 @@
       <c r="M24" s="17" t="s">
         <v>553</v>
       </c>
-      <c r="N24" s="57" t="s">
-        <v>702</v>
+      <c r="N24" s="56" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -15312,8 +15308,8 @@
       <c r="J25" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="K25" s="57" t="s">
-        <v>679</v>
+      <c r="K25" s="56" t="s">
+        <v>676</v>
       </c>
       <c r="L25" s="41" t="s">
         <v>480</v>
@@ -15321,8 +15317,8 @@
       <c r="M25" s="17" t="s">
         <v>553</v>
       </c>
-      <c r="N25" s="57" t="s">
-        <v>702</v>
+      <c r="N25" s="56" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -15354,15 +15350,15 @@
       <c r="J26" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="K26" s="57" t="s">
-        <v>679</v>
+      <c r="K26" s="56" t="s">
+        <v>676</v>
       </c>
       <c r="L26" s="41" t="s">
         <v>480</v>
       </c>
       <c r="M26" s="14"/>
-      <c r="N26" s="57" t="s">
-        <v>702</v>
+      <c r="N26" s="56" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -15396,8 +15392,8 @@
       <c r="J27" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="K27" s="57" t="s">
-        <v>679</v>
+      <c r="K27" s="56" t="s">
+        <v>676</v>
       </c>
       <c r="L27" s="41" t="s">
         <v>480</v>
@@ -15405,8 +15401,8 @@
       <c r="M27" s="17" t="s">
         <v>553</v>
       </c>
-      <c r="N27" s="57" t="s">
-        <v>702</v>
+      <c r="N27" s="56" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -15440,8 +15436,8 @@
       <c r="J28" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="K28" s="57" t="s">
-        <v>679</v>
+      <c r="K28" s="56" t="s">
+        <v>676</v>
       </c>
       <c r="L28" s="41" t="s">
         <v>480</v>
@@ -15449,8 +15445,8 @@
       <c r="M28" s="17" t="s">
         <v>553</v>
       </c>
-      <c r="N28" s="57" t="s">
-        <v>702</v>
+      <c r="N28" s="56" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -15482,15 +15478,15 @@
       <c r="J29" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="K29" s="57" t="s">
-        <v>679</v>
+      <c r="K29" s="56" t="s">
+        <v>676</v>
       </c>
       <c r="L29" s="41" t="s">
         <v>475</v>
       </c>
       <c r="M29" s="14"/>
-      <c r="N29" s="57" t="s">
-        <v>702</v>
+      <c r="N29" s="56" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -15524,7 +15520,7 @@
       <c r="J30" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="K30" s="57" t="s">
+      <c r="K30" s="56" t="s">
         <v>550</v>
       </c>
       <c r="L30" s="41" t="s">
@@ -15533,8 +15529,8 @@
       <c r="M30" s="14" t="s">
         <v>475</v>
       </c>
-      <c r="N30" s="57" t="s">
-        <v>703</v>
+      <c r="N30" s="56" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -15568,8 +15564,8 @@
       <c r="J31" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="K31" s="57" t="s">
-        <v>679</v>
+      <c r="K31" s="56" t="s">
+        <v>676</v>
       </c>
       <c r="L31" s="41" t="s">
         <v>475</v>
@@ -15577,8 +15573,8 @@
       <c r="M31" s="17" t="s">
         <v>553</v>
       </c>
-      <c r="N31" s="57" t="s">
-        <v>702</v>
+      <c r="N31" s="56" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -15622,7 +15618,7 @@
         <v>475</v>
       </c>
       <c r="N32" s="17" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -15666,7 +15662,7 @@
         <v>475</v>
       </c>
       <c r="N33" s="17" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -15710,7 +15706,7 @@
         <v>475</v>
       </c>
       <c r="N34" s="17" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -15754,7 +15750,7 @@
         <v>554</v>
       </c>
       <c r="N35" s="17" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -15798,7 +15794,7 @@
         <v>554</v>
       </c>
       <c r="N36" s="17" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -15842,7 +15838,7 @@
         <v>554</v>
       </c>
       <c r="N37" s="17" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -15886,7 +15882,7 @@
         <v>554</v>
       </c>
       <c r="N38" s="17" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -15930,7 +15926,7 @@
         <v>554</v>
       </c>
       <c r="N39" s="17" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -15974,7 +15970,7 @@
         <v>554</v>
       </c>
       <c r="N40" s="17" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -16018,7 +16014,7 @@
         <v>554</v>
       </c>
       <c r="N41" s="17" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -16062,7 +16058,7 @@
         <v>554</v>
       </c>
       <c r="N42" s="17" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -16106,7 +16102,7 @@
         <v>554</v>
       </c>
       <c r="N43" s="17" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -16150,7 +16146,7 @@
         <v>554</v>
       </c>
       <c r="N44" s="17" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -16194,7 +16190,7 @@
         <v>554</v>
       </c>
       <c r="N45" s="17" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -16345,8 +16341,8 @@
       <c r="J49" s="17" t="s">
         <v>549</v>
       </c>
-      <c r="K49" s="57" t="s">
-        <v>676</v>
+      <c r="K49" s="56" t="s">
+        <v>673</v>
       </c>
       <c r="L49" s="41" t="s">
         <v>475</v>
@@ -16354,7 +16350,7 @@
       <c r="M49" s="14" t="s">
         <v>475</v>
       </c>
-      <c r="N49" s="57" t="s">
+      <c r="N49" s="56" t="s">
         <v>383</v>
       </c>
     </row>
@@ -16389,8 +16385,8 @@
       <c r="J50" s="17" t="s">
         <v>549</v>
       </c>
-      <c r="K50" s="57" t="s">
-        <v>676</v>
+      <c r="K50" s="56" t="s">
+        <v>673</v>
       </c>
       <c r="L50" s="41" t="s">
         <v>475</v>
@@ -16398,7 +16394,7 @@
       <c r="M50" s="14" t="s">
         <v>475</v>
       </c>
-      <c r="N50" s="57" t="s">
+      <c r="N50" s="56" t="s">
         <v>383</v>
       </c>
     </row>
@@ -16433,8 +16429,8 @@
       <c r="J51" s="17" t="s">
         <v>549</v>
       </c>
-      <c r="K51" s="57" t="s">
-        <v>676</v>
+      <c r="K51" s="56" t="s">
+        <v>673</v>
       </c>
       <c r="L51" s="41" t="s">
         <v>475</v>
@@ -16442,7 +16438,7 @@
       <c r="M51" s="14" t="s">
         <v>475</v>
       </c>
-      <c r="N51" s="57" t="s">
+      <c r="N51" s="56" t="s">
         <v>383</v>
       </c>
     </row>
@@ -16477,8 +16473,8 @@
       <c r="J52" s="17" t="s">
         <v>549</v>
       </c>
-      <c r="K52" s="57" t="s">
-        <v>676</v>
+      <c r="K52" s="56" t="s">
+        <v>673</v>
       </c>
       <c r="L52" s="41" t="s">
         <v>475</v>
@@ -16486,7 +16482,7 @@
       <c r="M52" s="14" t="s">
         <v>475</v>
       </c>
-      <c r="N52" s="57" t="s">
+      <c r="N52" s="56" t="s">
         <v>383</v>
       </c>
     </row>
@@ -16521,8 +16517,8 @@
       <c r="J53" s="17" t="s">
         <v>549</v>
       </c>
-      <c r="K53" s="57" t="s">
-        <v>676</v>
+      <c r="K53" s="56" t="s">
+        <v>673</v>
       </c>
       <c r="L53" s="41" t="s">
         <v>475</v>
@@ -16530,7 +16526,7 @@
       <c r="M53" s="14" t="s">
         <v>475</v>
       </c>
-      <c r="N53" s="57" t="s">
+      <c r="N53" s="56" t="s">
         <v>383</v>
       </c>
     </row>
@@ -16776,7 +16772,7 @@
       <c r="L60" s="14"/>
       <c r="M60" s="14"/>
       <c r="N60" s="14" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
     </row>
     <row r="61" spans="1:14">
@@ -16811,7 +16807,7 @@
       <c r="L61" s="14"/>
       <c r="M61" s="14"/>
       <c r="N61" s="14" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
     </row>
     <row r="62" spans="1:14">
@@ -16846,7 +16842,7 @@
       <c r="L62" s="14"/>
       <c r="M62" s="14"/>
       <c r="N62" s="14" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
     </row>
     <row r="63" spans="1:14">
@@ -16881,7 +16877,7 @@
       <c r="L63" s="14"/>
       <c r="M63" s="14"/>
       <c r="N63" s="14" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
     </row>
     <row r="64" spans="1:14">
@@ -16951,8 +16947,8 @@
       <c r="J65" s="14" t="s">
         <v>462</v>
       </c>
-      <c r="K65" s="57" t="s">
-        <v>679</v>
+      <c r="K65" s="56" t="s">
+        <v>676</v>
       </c>
       <c r="L65" s="41" t="s">
         <v>475</v>
@@ -16960,8 +16956,8 @@
       <c r="M65" s="17" t="s">
         <v>553</v>
       </c>
-      <c r="N65" s="57" t="s">
-        <v>702</v>
+      <c r="N65" s="56" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="66" spans="1:14">
@@ -17005,7 +17001,7 @@
         <v>484</v>
       </c>
       <c r="N66" s="45" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
     </row>
     <row r="67" spans="1:14">
@@ -17049,7 +17045,7 @@
         <v>484</v>
       </c>
       <c r="N67" s="45" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
     </row>
     <row r="68" spans="1:14">
@@ -17093,7 +17089,7 @@
         <v>484</v>
       </c>
       <c r="N68" s="45" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
     </row>
     <row r="69" spans="1:14">
@@ -18725,7 +18721,7 @@
         <v>552</v>
       </c>
       <c r="N110" s="39" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
     </row>
     <row r="111" spans="1:14">
@@ -18769,7 +18765,7 @@
         <v>552</v>
       </c>
       <c r="N111" s="39" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
     </row>
     <row r="112" spans="1:14">
@@ -19236,7 +19232,7 @@
         <v>484</v>
       </c>
       <c r="N122" s="45" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
     </row>
     <row r="123" spans="1:14">
@@ -19381,7 +19377,7 @@
         <v>485</v>
       </c>
       <c r="K1" s="33" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="L1" s="33" t="s">
         <v>486</v>
@@ -19393,7 +19389,7 @@
         <v>488</v>
       </c>
       <c r="O1" s="33" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -20500,7 +20496,7 @@
         <f>VLOOKUP($B22,items_german!$B$2:$M$124,9,FALSE)</f>
         <v>Ölfrüchte</v>
       </c>
-      <c r="L22" s="57" t="str">
+      <c r="L22" s="56" t="str">
         <f>VLOOKUP($B22,items_german!$B$2:$M$124,10,FALSE)</f>
         <v>Hülsenfrüchte</v>
       </c>
@@ -20512,7 +20508,7 @@
         <f>VLOOKUP($B22,items_german!$B$2:$M$124,12,FALSE)</f>
         <v>Nüsse, Ölsaaten &amp; Hülsenfrüchte</v>
       </c>
-      <c r="O22" s="57" t="str">
+      <c r="O22" s="56" t="str">
         <f>VLOOKUP($B22,items_german!$B$2:$N$124,13,FALSE)</f>
         <v>Legumes</v>
       </c>
@@ -20551,8 +20547,8 @@
       <c r="K23" s="42" t="s">
         <v>462</v>
       </c>
-      <c r="L23" s="57" t="s">
-        <v>679</v>
+      <c r="L23" s="56" t="s">
+        <v>676</v>
       </c>
       <c r="M23" s="42" t="s">
         <v>480</v>
@@ -20560,8 +20556,8 @@
       <c r="N23" s="42" t="s">
         <v>483</v>
       </c>
-      <c r="O23" s="57" t="s">
-        <v>702</v>
+      <c r="O23" s="56" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -22816,7 +22812,7 @@
         <v>484</v>
       </c>
       <c r="O67" s="45" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
     </row>
     <row r="68" spans="1:15">
@@ -22863,7 +22859,7 @@
         <v>484</v>
       </c>
       <c r="O68" s="45" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
     </row>
     <row r="69" spans="1:15">
@@ -26000,30 +25996,30 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="C4" s="43" t="s">
         <v>674</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>658</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>677</v>
-      </c>
     </row>
     <row r="5" spans="1:4" ht="15.75">
-      <c r="A5" s="57" t="s">
-        <v>679</v>
+      <c r="A5" s="56" t="s">
+        <v>676</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>702</v>
+        <v>695</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="D5" s="44"/>
     </row>
     <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="14" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>57</v>
@@ -26037,10 +26033,10 @@
         <v>550</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75">
@@ -26059,7 +26055,7 @@
         <v>465</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
       <c r="C9" s="44" t="s">
         <v>562</v>
@@ -26070,7 +26066,7 @@
         <v>419</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
       <c r="C10" s="44" t="s">
         <v>562</v>
@@ -26081,7 +26077,7 @@
         <v>466</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
       <c r="C11" s="44" t="s">
         <v>562</v>
@@ -26136,7 +26132,7 @@
         <v>552</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
       <c r="C16" s="44" t="s">
         <v>564</v>
@@ -26188,13 +26184,13 @@
     </row>
     <row r="21" spans="1:4" ht="15.75">
       <c r="A21" s="14" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>383</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75">
@@ -26213,7 +26209,7 @@
         <v>570</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
       <c r="C23" s="44" t="s">
         <v>559</v>
@@ -26228,7 +26224,7 @@
         <v>206</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -26294,29 +26290,29 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="C4" s="43" t="s">
         <v>674</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>658</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>677</v>
-      </c>
     </row>
     <row r="5" spans="1:3" ht="15.75">
-      <c r="A5" s="57" t="s">
-        <v>679</v>
+      <c r="A5" s="56" t="s">
+        <v>676</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>702</v>
+        <v>695</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75">
       <c r="A6" s="14" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>57</v>
@@ -26330,10 +26326,10 @@
         <v>550</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75">
@@ -26352,7 +26348,7 @@
         <v>465</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
       <c r="C9" s="44" t="s">
         <v>562</v>
@@ -26363,7 +26359,7 @@
         <v>419</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
       <c r="C10" s="44" t="s">
         <v>562</v>
@@ -26374,7 +26370,7 @@
         <v>466</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
       <c r="C11" s="44" t="s">
         <v>562</v>
@@ -26429,7 +26425,7 @@
         <v>552</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
       <c r="C16" s="44" t="s">
         <v>564</v>
@@ -26481,13 +26477,13 @@
     </row>
     <row r="21" spans="1:6" ht="15.75">
       <c r="A21" s="14" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>383</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75">
@@ -26506,10 +26502,10 @@
         <v>570</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
       <c r="C23" s="44" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="F23"/>
     </row>
@@ -26521,7 +26517,7 @@
         <v>206</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="F24"/>
     </row>
@@ -26851,13 +26847,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="69" t="s">
         <v>322</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="18" t="s">
@@ -26882,7 +26878,7 @@
         <v>371</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>361</v>
@@ -27304,7 +27300,7 @@
         <v>347</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -27336,7 +27332,7 @@
         <v>347</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>698</v>
+        <v>691</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -27400,7 +27396,7 @@
         <v>347</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -27536,7 +27532,7 @@
         <v>300</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="C23" s="23" t="s">
         <v>358</v>
@@ -27575,8 +27571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B17" sqref="A15:B17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
@@ -27592,7 +27588,7 @@
     <col min="12" max="12" width="8.85546875" style="14" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" style="14" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="10.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34" style="14" customWidth="1"/>
+    <col min="15" max="15" width="45.7109375" style="14" customWidth="1"/>
     <col min="16" max="16" width="16.85546875" style="14" customWidth="1"/>
     <col min="17" max="17" width="18.140625" style="14" customWidth="1"/>
     <col min="18" max="18" width="74.42578125" style="14" bestFit="1" customWidth="1"/>
@@ -27600,62 +27596,62 @@
     <col min="20" max="16384" width="9.28515625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="53" customFormat="1">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:20" s="52" customFormat="1">
+      <c r="A1" s="52" t="s">
+        <v>657</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>602</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>658</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>601</v>
+      </c>
+      <c r="E1" s="52" t="s">
+        <v>654</v>
+      </c>
+      <c r="F1" s="52" t="s">
         <v>660</v>
       </c>
-      <c r="B1" s="53" t="s">
-        <v>602</v>
-      </c>
-      <c r="C1" s="53" t="s">
+      <c r="G1" s="52" t="s">
         <v>661</v>
       </c>
-      <c r="D1" s="53" t="s">
-        <v>601</v>
-      </c>
-      <c r="E1" s="53" t="s">
-        <v>657</v>
-      </c>
-      <c r="F1" s="53" t="s">
-        <v>663</v>
-      </c>
-      <c r="G1" s="53" t="s">
-        <v>664</v>
-      </c>
-      <c r="H1" s="53" t="s">
-        <v>665</v>
-      </c>
-      <c r="I1" s="53" t="s">
-        <v>654</v>
-      </c>
-      <c r="J1" s="53" t="s">
+      <c r="H1" s="52" t="s">
+        <v>662</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>651</v>
+      </c>
+      <c r="J1" s="52" t="s">
         <v>622</v>
       </c>
-      <c r="K1" s="53" t="s">
-        <v>634</v>
-      </c>
-      <c r="L1" s="53" t="s">
+      <c r="K1" s="52" t="s">
+        <v>633</v>
+      </c>
+      <c r="L1" s="52" t="s">
         <v>581</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="52" t="s">
         <v>573</v>
       </c>
-      <c r="N1" s="53" t="s">
+      <c r="N1" s="52" t="s">
         <v>325</v>
       </c>
-      <c r="O1" s="53" t="s">
+      <c r="O1" s="52" t="s">
         <v>596</v>
       </c>
-      <c r="P1" s="53" t="s">
+      <c r="P1" s="52" t="s">
         <v>591</v>
       </c>
-      <c r="Q1" s="53" t="s">
-        <v>655</v>
-      </c>
-      <c r="R1" s="53" t="s">
+      <c r="Q1" s="52" t="s">
+        <v>652</v>
+      </c>
+      <c r="R1" s="52" t="s">
         <v>594</v>
       </c>
-      <c r="S1" s="53" t="s">
+      <c r="S1" s="52" t="s">
         <v>592</v>
       </c>
     </row>
@@ -27681,10 +27677,10 @@
       <c r="G2" s="14">
         <v>1</v>
       </c>
-      <c r="H2" s="51">
+      <c r="H2" s="50">
         <v>50</v>
       </c>
-      <c r="I2" s="51">
+      <c r="I2" s="50">
         <v>50</v>
       </c>
       <c r="J2" s="14" t="s">
@@ -27695,11 +27691,12 @@
       </c>
       <c r="L2" s="48"/>
       <c r="M2" s="48"/>
-      <c r="N2" s="48">
+      <c r="N2" s="61">
+        <f>epo_overview!G2*epo_overview!K2</f>
         <v>50</v>
       </c>
-      <c r="O2" s="63" t="s">
-        <v>631</v>
+      <c r="O2" s="62" t="s">
+        <v>630</v>
       </c>
       <c r="S2" s="33"/>
       <c r="T2" s="33"/>
@@ -27720,44 +27717,44 @@
       <c r="E3" s="14" t="s">
         <v>608</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="50" t="s">
+        <v>614</v>
+      </c>
+      <c r="G3" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="H3" s="53" t="s">
+        <v>701</v>
+      </c>
+      <c r="I3" s="68">
         <v>1</v>
-      </c>
-      <c r="G3" s="14">
-        <v>1</v>
-      </c>
-      <c r="H3" s="54" t="s">
-        <v>614</v>
-      </c>
-      <c r="I3" s="54" t="s">
-        <v>629</v>
       </c>
       <c r="J3" s="36" t="s">
         <v>615</v>
       </c>
-      <c r="K3" s="58">
+      <c r="K3" s="57">
         <f>I3*P3</f>
-        <v>20.25</v>
-      </c>
-      <c r="L3" s="61"/>
+        <v>13.5</v>
+      </c>
+      <c r="L3" s="60"/>
       <c r="M3" s="48" t="s">
         <v>574</v>
       </c>
-      <c r="N3" s="62">
-        <f>I3*P3</f>
+      <c r="N3" s="61">
+        <f>epo_overview!G3*epo_overview!K3</f>
         <v>20.25</v>
       </c>
       <c r="O3" s="33" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="P3" s="33">
         <v>13.5</v>
       </c>
       <c r="Q3" s="14" t="s">
+        <v>631</v>
+      </c>
+      <c r="R3" s="14" t="s">
         <v>632</v>
-      </c>
-      <c r="R3" s="14" t="s">
-        <v>633</v>
       </c>
       <c r="S3" s="33"/>
       <c r="T3" s="33"/>
@@ -27784,10 +27781,10 @@
       <c r="G4" s="33">
         <v>1</v>
       </c>
-      <c r="H4" s="56">
+      <c r="H4" s="55">
         <v>22.5</v>
       </c>
-      <c r="I4" s="56">
+      <c r="I4" s="55">
         <v>22.5</v>
       </c>
       <c r="J4" s="33" t="s">
@@ -27796,15 +27793,16 @@
       <c r="K4" s="33">
         <v>22.5</v>
       </c>
-      <c r="L4" s="61"/>
+      <c r="L4" s="60"/>
       <c r="M4" s="48" t="s">
         <v>577</v>
       </c>
-      <c r="N4" s="48">
+      <c r="N4" s="61">
+        <f>epo_overview!G4*epo_overview!K4</f>
         <v>22.5</v>
       </c>
       <c r="O4" s="33" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -27823,17 +27821,17 @@
       <c r="E5" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="50" t="s">
         <v>612</v>
       </c>
       <c r="G5" s="49">
         <f>2/7</f>
         <v>0.2857142857142857</v>
       </c>
-      <c r="H5" s="56">
+      <c r="H5" s="55">
         <v>150</v>
       </c>
-      <c r="I5" s="56">
+      <c r="I5" s="55">
         <v>150</v>
       </c>
       <c r="J5" s="36" t="s">
@@ -27847,8 +27845,8 @@
         <v>300</v>
       </c>
       <c r="M5" s="48"/>
-      <c r="N5" s="50">
-        <f>G5*K5</f>
+      <c r="N5" s="74">
+        <f>epo_overview!G5*epo_overview!K5</f>
         <v>42.857142857142854</v>
       </c>
       <c r="O5" s="14" t="s">
@@ -27871,17 +27869,17 @@
       <c r="E6" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="F6" s="51" t="s">
+      <c r="F6" s="50" t="s">
         <v>613</v>
       </c>
       <c r="G6" s="49">
         <f>3/7</f>
         <v>0.42857142857142855</v>
       </c>
-      <c r="H6" s="56">
+      <c r="H6" s="55">
         <v>1</v>
       </c>
-      <c r="I6" s="56">
+      <c r="I6" s="55">
         <v>1</v>
       </c>
       <c r="J6" s="36" t="s">
@@ -27895,12 +27893,12 @@
         <v>174</v>
       </c>
       <c r="M6" s="48"/>
-      <c r="N6" s="50">
-        <f>K6*G6</f>
+      <c r="N6" s="74">
+        <f>epo_overview!G6*epo_overview!K6</f>
         <v>24.857142857142854</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="P6" s="14">
         <v>58</v>
@@ -27931,37 +27929,37 @@
       <c r="E7" s="14" t="s">
         <v>606</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="F7" s="50" t="s">
         <v>613</v>
       </c>
       <c r="G7" s="49">
-        <f>3/7</f>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="H7" s="51">
-        <v>150</v>
-      </c>
-      <c r="I7" s="51">
-        <v>150</v>
+        <f>2/7</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="H7" s="50" t="s">
+        <v>704</v>
+      </c>
+      <c r="I7" s="50">
+        <v>125</v>
       </c>
       <c r="J7" s="36" t="s">
         <v>623</v>
       </c>
       <c r="K7" s="36">
         <f>I7</f>
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="L7" s="48">
-        <f>I7*3</f>
-        <v>450</v>
+        <f>I7*2</f>
+        <v>250</v>
       </c>
       <c r="M7" s="48"/>
-      <c r="N7" s="50">
-        <f>K7*G7</f>
-        <v>64.285714285714278</v>
+      <c r="N7" s="74">
+        <f>epo_overview!G7*epo_overview!K7</f>
+        <v>35.714285714285715</v>
       </c>
       <c r="O7" s="33" t="s">
-        <v>638</v>
+        <v>702</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -27980,37 +27978,37 @@
       <c r="E8" s="14" t="s">
         <v>607</v>
       </c>
-      <c r="F8" s="56" t="s">
-        <v>636</v>
-      </c>
-      <c r="G8" s="59">
+      <c r="F8" s="55" t="s">
+        <v>635</v>
+      </c>
+      <c r="G8" s="58">
         <f>1/7</f>
         <v>0.14285714285714285</v>
       </c>
-      <c r="H8" s="60">
-        <v>150</v>
-      </c>
-      <c r="I8" s="60">
-        <v>150</v>
+      <c r="H8" s="50" t="s">
+        <v>704</v>
+      </c>
+      <c r="I8" s="59">
+        <v>125</v>
       </c>
       <c r="J8" s="33" t="s">
         <v>623</v>
       </c>
       <c r="K8" s="36">
-        <f>H8</f>
-        <v>150</v>
+        <f>I8</f>
+        <v>125</v>
       </c>
       <c r="L8" s="48">
         <f>1*K8</f>
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="M8" s="48"/>
-      <c r="N8" s="50">
-        <f>G8*K8</f>
-        <v>21.428571428571427</v>
+      <c r="N8" s="74">
+        <f>epo_overview!G8*epo_overview!K8</f>
+        <v>17.857142857142858</v>
       </c>
       <c r="O8" s="33" t="s">
-        <v>637</v>
+        <v>703</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -28029,16 +28027,16 @@
       <c r="E9" s="14" t="s">
         <v>603</v>
       </c>
-      <c r="F9" s="51">
+      <c r="F9" s="50">
         <v>4</v>
       </c>
       <c r="G9" s="14">
         <v>4</v>
       </c>
-      <c r="H9" s="51">
+      <c r="H9" s="50">
         <v>200</v>
       </c>
-      <c r="I9" s="51">
+      <c r="I9" s="50">
         <v>200</v>
       </c>
       <c r="J9" s="14" t="s">
@@ -28052,12 +28050,12 @@
       <c r="M9" s="48" t="s">
         <v>586</v>
       </c>
-      <c r="N9" s="48">
-        <f>K9*G9</f>
+      <c r="N9" s="75">
+        <f>epo_overview!G9*epo_overview!K9</f>
         <v>824</v>
       </c>
       <c r="O9" s="33" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="P9" s="14">
         <v>1.03</v>
@@ -28085,16 +28083,16 @@
       <c r="E10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="55">
+      <c r="F10" s="54">
         <v>4</v>
       </c>
       <c r="G10" s="46">
         <v>4</v>
       </c>
-      <c r="H10" s="51" t="s">
+      <c r="H10" s="50" t="s">
         <v>626</v>
       </c>
-      <c r="I10" s="51">
+      <c r="I10" s="50">
         <v>55</v>
       </c>
       <c r="J10" s="14" t="s">
@@ -28126,16 +28124,16 @@
       <c r="E11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="55">
+      <c r="F11" s="54">
         <v>4</v>
       </c>
       <c r="G11" s="46">
         <v>4</v>
       </c>
-      <c r="H11" s="51" t="s">
+      <c r="H11" s="50" t="s">
         <v>627</v>
       </c>
-      <c r="I11" s="51">
+      <c r="I11" s="50">
         <v>225</v>
       </c>
       <c r="J11" s="14" t="s">
@@ -28151,7 +28149,7 @@
         <v>620</v>
       </c>
       <c r="O11" s="33" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="P11" s="33"/>
       <c r="Q11" s="33"/>
@@ -28163,7 +28161,7 @@
         <v>587</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="C12" s="36" t="s">
         <v>590</v>
@@ -28174,16 +28172,16 @@
       <c r="E12" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="F12" s="55">
+      <c r="F12" s="54">
         <v>3</v>
       </c>
       <c r="G12" s="46">
         <v>3</v>
       </c>
-      <c r="H12" s="51" t="s">
+      <c r="H12" s="50" t="s">
         <v>617</v>
       </c>
-      <c r="I12" s="51">
+      <c r="I12" s="50">
         <v>150</v>
       </c>
       <c r="J12" s="14" t="s">
@@ -28208,7 +28206,7 @@
         <v>587</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>589</v>
@@ -28217,18 +28215,18 @@
         <v>610</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>658</v>
-      </c>
-      <c r="F13" s="55">
+        <v>655</v>
+      </c>
+      <c r="F13" s="54">
         <v>3</v>
       </c>
       <c r="G13" s="46">
         <v>3</v>
       </c>
-      <c r="H13" s="51" t="s">
+      <c r="H13" s="50" t="s">
         <v>628</v>
       </c>
-      <c r="I13" s="51">
+      <c r="I13" s="50">
         <f>(70+100)/2</f>
         <v>85</v>
       </c>
@@ -28265,16 +28263,16 @@
       <c r="E14" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="F14" s="51">
+      <c r="F14" s="50">
         <v>2</v>
       </c>
       <c r="G14" s="14">
         <v>2</v>
       </c>
-      <c r="H14" s="51" t="s">
+      <c r="H14" s="50" t="s">
         <v>616</v>
       </c>
-      <c r="I14" s="51">
+      <c r="I14" s="50">
         <f>(125+150)/2</f>
         <v>137.5</v>
       </c>
@@ -28287,12 +28285,12 @@
       </c>
       <c r="L14" s="48"/>
       <c r="M14" s="48"/>
-      <c r="N14" s="48">
-        <f>K14*F14</f>
+      <c r="N14" s="75">
+        <f>epo_overview!G14*epo_overview!K14</f>
         <v>275</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="P14" s="33"/>
       <c r="Q14" s="33"/>
@@ -28301,34 +28299,34 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="14" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>518</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>611</v>
       </c>
-      <c r="F15" s="65" t="s">
+      <c r="F15" s="64" t="s">
         <v>358</v>
       </c>
-      <c r="G15" s="66" t="s">
+      <c r="G15" s="65" t="s">
         <v>358</v>
       </c>
       <c r="H15" s="33">
         <v>1</v>
       </c>
-      <c r="I15" s="60">
+      <c r="I15" s="59">
         <v>1</v>
       </c>
       <c r="J15" s="33" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="K15" s="33">
         <v>7</v>
@@ -28336,10 +28334,10 @@
       <c r="L15" s="48"/>
       <c r="M15" s="48"/>
       <c r="N15" s="48" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="O15" s="33" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="P15" s="33"/>
       <c r="Q15" s="33"/>
@@ -28348,34 +28346,34 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="14" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>520</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>659</v>
-      </c>
-      <c r="F16" s="65" t="s">
+        <v>656</v>
+      </c>
+      <c r="F16" s="64" t="s">
         <v>358</v>
       </c>
-      <c r="G16" s="66" t="s">
+      <c r="G16" s="65" t="s">
         <v>358</v>
       </c>
       <c r="H16" s="33">
         <v>1</v>
       </c>
-      <c r="I16" s="60">
+      <c r="I16" s="59">
         <v>1</v>
       </c>
       <c r="J16" s="33" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="K16" s="33">
         <v>3</v>
@@ -28383,10 +28381,10 @@
       <c r="L16" s="48"/>
       <c r="M16" s="48"/>
       <c r="N16" s="48" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="O16" s="33" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="P16" s="33"/>
       <c r="Q16" s="33"/>
@@ -28395,30 +28393,38 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="14" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>688</v>
-      </c>
-      <c r="F17" s="65" t="s">
+        <v>685</v>
+      </c>
+      <c r="F17" s="64" t="s">
         <v>358</v>
       </c>
-      <c r="G17" s="66" t="s">
+      <c r="G17" s="65" t="s">
         <v>358</v>
       </c>
-      <c r="H17" s="33"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
+      <c r="H17" s="33">
+        <v>1</v>
+      </c>
+      <c r="I17" s="59">
+        <v>1</v>
+      </c>
+      <c r="J17" s="33" t="s">
+        <v>637</v>
+      </c>
+      <c r="K17" s="59">
+        <v>6</v>
+      </c>
       <c r="L17" s="48"/>
       <c r="M17" s="48"/>
       <c r="N17" s="48"/>
@@ -28436,18 +28442,18 @@
         <v>469</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>206</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>672</v>
-      </c>
-      <c r="F18" s="65" t="s">
+        <v>669</v>
+      </c>
+      <c r="F18" s="64" t="s">
         <v>358</v>
       </c>
-      <c r="G18" s="66" t="s">
+      <c r="G18" s="65" t="s">
         <v>358</v>
       </c>
       <c r="H18" s="33">
@@ -28465,12 +28471,12 @@
       </c>
       <c r="L18" s="48"/>
       <c r="M18" s="48"/>
-      <c r="N18" s="48" t="e">
-        <f>K18*G18</f>
+      <c r="N18" s="75" t="e">
+        <f>epo_overview!G18*epo_overview!K18</f>
         <v>#VALUE!</v>
       </c>
       <c r="O18" s="33" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="P18" s="14">
         <v>1.01</v>
@@ -28498,10 +28504,10 @@
       <c r="E19" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="F19" s="65" t="s">
+      <c r="F19" s="64" t="s">
         <v>358</v>
       </c>
-      <c r="G19" s="66" t="s">
+      <c r="G19" s="65" t="s">
         <v>358</v>
       </c>
       <c r="H19" s="33">
@@ -28519,12 +28525,12 @@
       </c>
       <c r="L19" s="48"/>
       <c r="M19" s="48"/>
-      <c r="N19" s="48" t="e">
-        <f>K19*G18</f>
+      <c r="N19" s="75" t="e">
+        <f>epo_overview!G19*epo_overview!K19</f>
         <v>#VALUE!</v>
       </c>
       <c r="O19" s="33" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="P19" s="14">
         <v>0.99</v>
@@ -28544,25 +28550,25 @@
         <v>469</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>206</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>670</v>
-      </c>
-      <c r="F20" s="65" t="s">
+        <v>667</v>
+      </c>
+      <c r="F20" s="64" t="s">
         <v>358</v>
       </c>
-      <c r="G20" s="66" t="s">
+      <c r="G20" s="65" t="s">
         <v>358</v>
       </c>
-      <c r="H20" s="67">
+      <c r="H20" s="66">
         <f>0.06</f>
         <v>0.06</v>
       </c>
-      <c r="I20" s="67">
+      <c r="I20" s="66">
         <f>H20*1000</f>
         <v>60</v>
       </c>
@@ -28575,12 +28581,12 @@
       </c>
       <c r="L20" s="48"/>
       <c r="M20" s="48"/>
-      <c r="N20" s="48" t="e">
-        <f>K20*G19</f>
+      <c r="N20" s="75" t="e">
+        <f>epo_overview!G20*epo_overview!K20</f>
         <v>#VALUE!</v>
       </c>
       <c r="O20" s="33" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="P20" s="14">
         <v>0.95</v>
@@ -28594,13 +28600,13 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" s="33" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="D21" s="33" t="s">
         <v>383</v>
@@ -28608,22 +28614,25 @@
       <c r="E21" s="33" t="s">
         <v>383</v>
       </c>
-      <c r="F21" s="65" t="s">
+      <c r="F21" s="64" t="s">
         <v>358</v>
       </c>
-      <c r="G21" s="66" t="s">
+      <c r="G21" s="65" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="52"/>
-      <c r="B22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
+      <c r="A22" s="51"/>
+      <c r="B22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="G6 K9" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -28632,7 +28641,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
@@ -28643,15 +28652,15 @@
     <col min="4" max="16384" width="9.28515625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="53" customFormat="1">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:3" s="52" customFormat="1">
+      <c r="A1" s="52" t="s">
         <v>602</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="52" t="s">
         <v>601</v>
       </c>
-      <c r="C1" s="53" t="s">
-        <v>635</v>
+      <c r="C1" s="52" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -28662,6 +28671,7 @@
         <v>298</v>
       </c>
       <c r="C2" s="14">
+        <f>epo_overview!G2</f>
         <v>1</v>
       </c>
     </row>
@@ -28673,7 +28683,8 @@
         <v>608</v>
       </c>
       <c r="C3" s="14">
-        <v>1</v>
+        <f>epo_overview!G3</f>
+        <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -28683,7 +28694,8 @@
       <c r="B4" s="14" t="s">
         <v>609</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="73">
+        <f>epo_overview!G4</f>
         <v>1</v>
       </c>
     </row>
@@ -28695,7 +28707,7 @@
         <v>283</v>
       </c>
       <c r="C5" s="49">
-        <f>2/7</f>
+        <f>epo_overview!G5</f>
         <v>0.2857142857142857</v>
       </c>
     </row>
@@ -28707,7 +28719,7 @@
         <v>255</v>
       </c>
       <c r="C6" s="49">
-        <f>3/7</f>
+        <f>epo_overview!G6</f>
         <v>0.42857142857142855</v>
       </c>
     </row>
@@ -28719,8 +28731,8 @@
         <v>606</v>
       </c>
       <c r="C7" s="49">
-        <f>3/7</f>
-        <v>0.42857142857142855</v>
+        <f>epo_overview!G7</f>
+        <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -28730,8 +28742,8 @@
       <c r="B8" s="14" t="s">
         <v>607</v>
       </c>
-      <c r="C8" s="59">
-        <f>1/7</f>
+      <c r="C8" s="49">
+        <f>epo_overview!G8</f>
         <v>0.14285714285714285</v>
       </c>
     </row>
@@ -28742,7 +28754,8 @@
       <c r="B9" s="14" t="s">
         <v>603</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="73">
+        <f>epo_overview!G9</f>
         <v>4</v>
       </c>
     </row>
@@ -28753,18 +28766,20 @@
       <c r="B10" s="14" t="s">
         <v>604</v>
       </c>
-      <c r="C10" s="46">
+      <c r="C10" s="73">
+        <f>epo_overview!G10</f>
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="14" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>610</v>
       </c>
-      <c r="C11" s="46">
+      <c r="C11" s="73">
+        <f>epo_overview!G12</f>
         <v>3</v>
       </c>
     </row>
@@ -28775,18 +28790,19 @@
       <c r="B12" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="73">
+        <f>epo_overview!G14</f>
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="14" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>668</v>
-      </c>
-      <c r="C13" s="66" t="s">
+        <v>665</v>
+      </c>
+      <c r="C13" s="65" t="s">
         <v>358</v>
       </c>
     </row>
@@ -28797,7 +28813,7 @@
       <c r="B14" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="C14" s="66" t="s">
+      <c r="C14" s="65" t="s">
         <v>358</v>
       </c>
     </row>
@@ -28813,8 +28829,8 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="52"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="51"/>
+      <c r="B17" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28827,7 +28843,7 @@
   <dimension ref="A1:L124"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
@@ -28842,36 +28858,36 @@
     <col min="11" max="16384" width="9.28515625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="53" customFormat="1">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:12" s="52" customFormat="1">
+      <c r="A1" s="52" t="s">
         <v>602</v>
       </c>
-      <c r="B1" s="53" t="s">
-        <v>661</v>
-      </c>
-      <c r="C1" s="53" t="s">
+      <c r="B1" s="52" t="s">
+        <v>658</v>
+      </c>
+      <c r="C1" s="52" t="s">
         <v>601</v>
       </c>
-      <c r="D1" s="53" t="s">
-        <v>657</v>
-      </c>
-      <c r="E1" s="53" t="s">
-        <v>665</v>
-      </c>
-      <c r="F1" s="53" t="s">
+      <c r="D1" s="52" t="s">
         <v>654</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="E1" s="52" t="s">
+        <v>662</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>651</v>
+      </c>
+      <c r="G1" s="52" t="s">
         <v>622</v>
       </c>
-      <c r="H1" s="53" t="s">
-        <v>634</v>
-      </c>
-      <c r="I1" s="53" t="s">
+      <c r="H1" s="52" t="s">
+        <v>633</v>
+      </c>
+      <c r="I1" s="52" t="s">
         <v>591</v>
       </c>
-      <c r="J1" s="53" t="s">
-        <v>655</v>
+      <c r="J1" s="52" t="s">
+        <v>652</v>
       </c>
       <c r="L1" s="33"/>
     </row>
@@ -28888,18 +28904,23 @@
       <c r="D2" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="E2" s="51">
+      <c r="E2" s="50">
+        <f>epo_overview!H2</f>
         <v>50</v>
       </c>
-      <c r="F2" s="51">
+      <c r="F2" s="50">
+        <f>epo_overview!I2</f>
         <v>50</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="H2" s="14">
+      <c r="G2" s="50" t="str">
+        <f>epo_overview!J2</f>
+        <v>g</v>
+      </c>
+      <c r="H2" s="50">
+        <f>epo_overview!K2</f>
         <v>50</v>
       </c>
+      <c r="I2" s="50"/>
       <c r="K2" s="33"/>
       <c r="L2" s="33"/>
     </row>
@@ -28916,24 +28937,27 @@
       <c r="D3" s="14" t="s">
         <v>608</v>
       </c>
-      <c r="E3" s="54" t="s">
-        <v>614</v>
-      </c>
-      <c r="F3" s="70">
-        <v>1.5</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>615</v>
-      </c>
-      <c r="H3" s="58">
-        <f>F3*I3</f>
-        <v>20.25</v>
+      <c r="E3" s="50" t="str">
+        <f>epo_overview!H3</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="50">
+        <f>epo_overview!I3</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="50" t="str">
+        <f>epo_overview!J3</f>
+        <v>tablespoon</v>
+      </c>
+      <c r="H3" s="50">
+        <f>epo_overview!K3</f>
+        <v>13.5</v>
       </c>
       <c r="I3" s="33">
         <v>13.5</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="K3" s="33"/>
       <c r="L3" s="36"/>
@@ -28951,16 +28975,20 @@
       <c r="D4" s="14" t="s">
         <v>609</v>
       </c>
-      <c r="E4" s="56">
+      <c r="E4" s="50">
+        <f>epo_overview!H4</f>
         <v>22.5</v>
       </c>
-      <c r="F4" s="56">
+      <c r="F4" s="50">
+        <f>epo_overview!I4</f>
         <v>22.5</v>
       </c>
-      <c r="G4" s="33" t="s">
-        <v>623</v>
-      </c>
-      <c r="H4" s="33">
+      <c r="G4" s="50" t="str">
+        <f>epo_overview!J4</f>
+        <v>g</v>
+      </c>
+      <c r="H4" s="50">
+        <f>epo_overview!K4</f>
         <v>22.5</v>
       </c>
       <c r="L4" s="33"/>
@@ -28978,17 +29006,20 @@
       <c r="D5" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="E5" s="56">
+      <c r="E5" s="50">
+        <f>epo_overview!H5</f>
         <v>150</v>
       </c>
-      <c r="F5" s="56">
+      <c r="F5" s="50">
+        <f>epo_overview!I5</f>
         <v>150</v>
       </c>
-      <c r="G5" s="36" t="s">
-        <v>623</v>
-      </c>
-      <c r="H5" s="36">
-        <f>E5</f>
+      <c r="G5" s="50" t="str">
+        <f>epo_overview!J5</f>
+        <v>g</v>
+      </c>
+      <c r="H5" s="50">
+        <f>epo_overview!K5</f>
         <v>150</v>
       </c>
       <c r="L5" s="33"/>
@@ -29006,16 +29037,20 @@
       <c r="D6" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="E6" s="56">
+      <c r="E6" s="50">
+        <f>epo_overview!H6</f>
         <v>1</v>
       </c>
-      <c r="F6" s="56">
+      <c r="F6" s="50">
+        <f>epo_overview!I6</f>
         <v>1</v>
       </c>
-      <c r="G6" s="36" t="s">
-        <v>624</v>
-      </c>
-      <c r="H6" s="36">
+      <c r="G6" s="50" t="str">
+        <f>epo_overview!J6</f>
+        <v>egg</v>
+      </c>
+      <c r="H6" s="50">
+        <f>epo_overview!K6</f>
         <v>58</v>
       </c>
       <c r="I6" s="14">
@@ -29039,18 +29074,21 @@
       <c r="D7" s="14" t="s">
         <v>606</v>
       </c>
-      <c r="E7" s="51">
-        <v>150</v>
-      </c>
-      <c r="F7" s="51">
-        <v>150</v>
-      </c>
-      <c r="G7" s="36" t="s">
-        <v>623</v>
-      </c>
-      <c r="H7" s="36">
-        <f>F7</f>
-        <v>150</v>
+      <c r="E7" s="50" t="str">
+        <f>epo_overview!H7</f>
+        <v>100-150</v>
+      </c>
+      <c r="F7" s="50">
+        <f>epo_overview!I7</f>
+        <v>125</v>
+      </c>
+      <c r="G7" s="50" t="str">
+        <f>epo_overview!J7</f>
+        <v>g</v>
+      </c>
+      <c r="H7" s="50">
+        <f>epo_overview!K7</f>
+        <v>125</v>
       </c>
       <c r="L7" s="33"/>
     </row>
@@ -29067,18 +29105,21 @@
       <c r="D8" s="14" t="s">
         <v>607</v>
       </c>
-      <c r="E8" s="60">
-        <v>150</v>
-      </c>
-      <c r="F8" s="60">
-        <v>150</v>
-      </c>
-      <c r="G8" s="33" t="s">
-        <v>623</v>
-      </c>
-      <c r="H8" s="36">
-        <f>E8</f>
-        <v>150</v>
+      <c r="E8" s="50" t="str">
+        <f>epo_overview!H8</f>
+        <v>100-150</v>
+      </c>
+      <c r="F8" s="50">
+        <f>epo_overview!I8</f>
+        <v>125</v>
+      </c>
+      <c r="G8" s="50" t="str">
+        <f>epo_overview!J8</f>
+        <v>g</v>
+      </c>
+      <c r="H8" s="50">
+        <f>epo_overview!K8</f>
+        <v>125</v>
       </c>
       <c r="L8" s="36"/>
     </row>
@@ -29095,17 +29136,20 @@
       <c r="D9" s="14" t="s">
         <v>603</v>
       </c>
-      <c r="E9" s="51">
+      <c r="E9" s="50">
+        <f>epo_overview!H9</f>
         <v>200</v>
       </c>
-      <c r="F9" s="51">
+      <c r="F9" s="50">
+        <f>epo_overview!I9</f>
         <v>200</v>
       </c>
-      <c r="G9" s="14" t="s">
-        <v>625</v>
-      </c>
-      <c r="H9" s="14">
-        <f>F9*I9</f>
+      <c r="G9" s="50" t="str">
+        <f>epo_overview!J9</f>
+        <v>ml</v>
+      </c>
+      <c r="H9" s="50">
+        <f>epo_overview!K9</f>
         <v>206</v>
       </c>
       <c r="I9" s="14">
@@ -29129,17 +29173,20 @@
       <c r="D10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="51" t="s">
-        <v>626</v>
-      </c>
-      <c r="F10" s="51">
+      <c r="E10" s="50" t="str">
+        <f>epo_overview!H10</f>
+        <v>50-60</v>
+      </c>
+      <c r="F10" s="50">
+        <f>epo_overview!I10</f>
         <v>55</v>
       </c>
-      <c r="G10" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="H10" s="14">
-        <f>F10</f>
+      <c r="G10" s="50" t="str">
+        <f>epo_overview!J10</f>
+        <v>g</v>
+      </c>
+      <c r="H10" s="50">
+        <f>epo_overview!K10</f>
         <v>55</v>
       </c>
       <c r="L10" s="33"/>
@@ -29157,17 +29204,20 @@
       <c r="D11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="51" t="s">
-        <v>693</v>
-      </c>
-      <c r="F11" s="51">
+      <c r="E11" s="50" t="str">
+        <f>epo_overview!H11</f>
+        <v>200 - 250</v>
+      </c>
+      <c r="F11" s="50">
+        <f>epo_overview!I11</f>
         <v>225</v>
       </c>
-      <c r="G11" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="H11" s="14">
-        <f t="shared" ref="H11:H14" si="0">F11</f>
+      <c r="G11" s="50" t="str">
+        <f>epo_overview!J11</f>
+        <v>g</v>
+      </c>
+      <c r="H11" s="50">
+        <f>epo_overview!K11</f>
         <v>225</v>
       </c>
       <c r="I11" s="33"/>
@@ -29176,7 +29226,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="14" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="B12" s="36" t="s">
         <v>590</v>
@@ -29187,17 +29237,20 @@
       <c r="D12" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="E12" s="51" t="s">
-        <v>694</v>
-      </c>
-      <c r="F12" s="51">
+      <c r="E12" s="50" t="str">
+        <f>epo_overview!H12</f>
+        <v>100 - 200</v>
+      </c>
+      <c r="F12" s="50">
+        <f>epo_overview!I12</f>
         <v>150</v>
       </c>
-      <c r="G12" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="H12" s="14">
-        <f t="shared" si="0"/>
+      <c r="G12" s="50" t="str">
+        <f>epo_overview!J12</f>
+        <v>g</v>
+      </c>
+      <c r="H12" s="50">
+        <f>epo_overview!K12</f>
         <v>150</v>
       </c>
       <c r="I12" s="33"/>
@@ -29206,7 +29259,7 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="14" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>589</v>
@@ -29215,20 +29268,22 @@
         <v>610</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>658</v>
-      </c>
-      <c r="E13" s="51" t="s">
-        <v>695</v>
-      </c>
-      <c r="F13" s="51">
-        <f>(70+100)/2</f>
+        <v>655</v>
+      </c>
+      <c r="E13" s="50" t="str">
+        <f>epo_overview!H13</f>
+        <v>70 - 100</v>
+      </c>
+      <c r="F13" s="50">
+        <f>epo_overview!I13</f>
         <v>85</v>
       </c>
-      <c r="G13" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="H13" s="14">
-        <f t="shared" si="0"/>
+      <c r="G13" s="50" t="str">
+        <f>epo_overview!J13</f>
+        <v>g</v>
+      </c>
+      <c r="H13" s="50">
+        <f>epo_overview!K13</f>
         <v>85</v>
       </c>
       <c r="I13" s="33"/>
@@ -29248,18 +29303,20 @@
       <c r="D14" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="E14" s="51" t="s">
-        <v>696</v>
-      </c>
-      <c r="F14" s="51">
-        <f>(125+150)/2</f>
+      <c r="E14" s="50" t="str">
+        <f>epo_overview!H14</f>
+        <v>125 - 150</v>
+      </c>
+      <c r="F14" s="50">
+        <f>epo_overview!I14</f>
         <v>137.5</v>
       </c>
-      <c r="G14" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="H14" s="14">
-        <f t="shared" si="0"/>
+      <c r="G14" s="50" t="str">
+        <f>epo_overview!J14</f>
+        <v>g</v>
+      </c>
+      <c r="H14" s="50">
+        <f>epo_overview!K14</f>
         <v>137.5</v>
       </c>
       <c r="I14" s="33"/>
@@ -29268,27 +29325,31 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="14" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>518</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>611</v>
       </c>
-      <c r="E15" s="33">
+      <c r="E15" s="50">
+        <f>epo_overview!H15</f>
         <v>1</v>
       </c>
-      <c r="F15" s="60">
+      <c r="F15" s="50">
+        <f>epo_overview!I15</f>
         <v>1</v>
       </c>
-      <c r="G15" s="33" t="s">
-        <v>640</v>
-      </c>
-      <c r="H15" s="33">
+      <c r="G15" s="50" t="str">
+        <f>epo_overview!J15</f>
+        <v>cup</v>
+      </c>
+      <c r="H15" s="50">
+        <f>epo_overview!K15</f>
         <v>7</v>
       </c>
       <c r="I15" s="33"/>
@@ -29297,27 +29358,31 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="14" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>520</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>659</v>
-      </c>
-      <c r="E16" s="33">
+        <v>656</v>
+      </c>
+      <c r="E16" s="50">
+        <f>epo_overview!H16</f>
         <v>1</v>
       </c>
-      <c r="F16" s="60">
+      <c r="F16" s="50">
+        <f>epo_overview!I16</f>
         <v>1</v>
       </c>
-      <c r="G16" s="33" t="s">
-        <v>640</v>
-      </c>
-      <c r="H16" s="33">
+      <c r="G16" s="50" t="str">
+        <f>epo_overview!J16</f>
+        <v>cup</v>
+      </c>
+      <c r="H16" s="50">
+        <f>epo_overview!K16</f>
         <v>3</v>
       </c>
       <c r="I16" s="33"/>
@@ -29326,28 +29391,32 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="14" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>688</v>
-      </c>
-      <c r="E17" s="60" t="s">
-        <v>358</v>
-      </c>
-      <c r="F17" s="60" t="s">
-        <v>358</v>
-      </c>
-      <c r="G17" s="60" t="s">
-        <v>358</v>
-      </c>
-      <c r="H17" s="60" t="s">
-        <v>358</v>
+        <v>685</v>
+      </c>
+      <c r="E17" s="50">
+        <f>epo_overview!H17</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="50">
+        <f>epo_overview!I17</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="50" t="str">
+        <f>epo_overview!J17</f>
+        <v>cup</v>
+      </c>
+      <c r="H17" s="50">
+        <f>epo_overview!K17</f>
+        <v>6</v>
       </c>
       <c r="I17" s="33"/>
       <c r="J17" s="33"/>
@@ -29358,25 +29427,28 @@
         <v>469</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>206</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>672</v>
-      </c>
-      <c r="E18" s="33">
+        <v>669</v>
+      </c>
+      <c r="E18" s="50">
+        <f>epo_overview!H18</f>
         <v>0.5</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="50">
+        <f>epo_overview!I18</f>
         <v>500</v>
       </c>
-      <c r="G18" s="33" t="s">
-        <v>625</v>
-      </c>
-      <c r="H18" s="33">
-        <f>F18*I18</f>
+      <c r="G18" s="50" t="str">
+        <f>epo_overview!J18</f>
+        <v>ml</v>
+      </c>
+      <c r="H18" s="50">
+        <f>epo_overview!K18</f>
         <v>505</v>
       </c>
       <c r="I18" s="14">
@@ -29400,17 +29472,20 @@
       <c r="D19" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E19" s="50">
+        <f>epo_overview!H19</f>
         <v>0.25</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="50">
+        <f>epo_overview!I19</f>
         <v>250</v>
       </c>
-      <c r="G19" s="33" t="s">
-        <v>625</v>
-      </c>
-      <c r="H19" s="33">
-        <f>F19*I19</f>
+      <c r="G19" s="50" t="str">
+        <f>epo_overview!J19</f>
+        <v>ml</v>
+      </c>
+      <c r="H19" s="50">
+        <f>epo_overview!K19</f>
         <v>247.5</v>
       </c>
       <c r="I19" s="14">
@@ -29426,24 +29501,28 @@
         <v>469</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>206</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>670</v>
-      </c>
-      <c r="E20" s="67">
+        <v>667</v>
+      </c>
+      <c r="E20" s="50">
+        <f>epo_overview!H20</f>
         <v>0.06</v>
       </c>
-      <c r="F20" s="68">
+      <c r="F20" s="50">
+        <f>epo_overview!I20</f>
         <v>60</v>
       </c>
-      <c r="G20" s="33" t="s">
-        <v>625</v>
-      </c>
-      <c r="H20" s="59">
+      <c r="G20" s="50" t="str">
+        <f>epo_overview!J20</f>
+        <v>ml</v>
+      </c>
+      <c r="H20" s="50">
+        <f>epo_overview!K20</f>
         <v>57</v>
       </c>
       <c r="I20" s="14">
@@ -29456,10 +29535,10 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="33" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="C21" s="33" t="s">
         <v>383</v>
@@ -29467,24 +29546,24 @@
       <c r="D21" s="33" t="s">
         <v>383</v>
       </c>
-      <c r="E21" s="65" t="s">
+      <c r="E21" s="64" t="s">
         <v>358</v>
       </c>
-      <c r="F21" s="60" t="s">
+      <c r="F21" s="59" t="s">
         <v>358</v>
       </c>
-      <c r="G21" s="60" t="s">
+      <c r="G21" s="59" t="s">
         <v>358</v>
       </c>
-      <c r="H21" s="60" t="s">
+      <c r="H21" s="59" t="s">
         <v>358</v>
       </c>
       <c r="L21"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
+      <c r="A22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
       <c r="L22"/>
     </row>
     <row r="23" spans="1:12">
@@ -29804,7 +29883,7 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F5" sqref="F5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -30585,7 +30664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -30612,13 +30691,13 @@
         <v>601</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="F1" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="G1" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -30639,7 +30718,7 @@
         <v>0.30699999999999994</v>
       </c>
       <c r="F2" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -30967,10 +31046,10 @@
         <v>0.5</v>
       </c>
       <c r="F21" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="G21" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -31007,7 +31086,7 @@
         <v>0.3</v>
       </c>
       <c r="F23" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -31159,10 +31238,10 @@
         <v>0.27</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G32" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -31182,10 +31261,10 @@
         <v>0.27</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -31205,10 +31284,10 @@
         <v>0.27</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -31228,7 +31307,7 @@
         <v>0.27</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -31248,7 +31327,7 @@
         <v>0.27</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -31268,7 +31347,7 @@
         <v>0.27</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -31288,7 +31367,7 @@
         <v>0.27</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -31308,7 +31387,7 @@
         <v>0.27</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -31328,7 +31407,7 @@
         <v>0.27</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -31348,7 +31427,7 @@
         <v>0.27</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -31368,7 +31447,7 @@
         <v>0.27</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -31388,7 +31467,7 @@
         <v>0.27</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -31408,7 +31487,7 @@
         <v>0.27</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -31428,7 +31507,7 @@
         <v>0.27</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -31448,7 +31527,7 @@
         <v>0.3</v>
       </c>
       <c r="F46" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -31468,7 +31547,7 @@
         <v>0.2</v>
       </c>
       <c r="F47" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -32538,9 +32617,9 @@
         <v>0.34</v>
       </c>
       <c r="F114" t="s">
-        <v>652</v>
-      </c>
-      <c r="G114" s="52"/>
+        <v>649</v>
+      </c>
+      <c r="G114" s="51"/>
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="14" t="s">
@@ -32559,7 +32638,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="F115" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -32579,7 +32658,7 @@
         <v>0.29499999999999998</v>
       </c>
       <c r="F116" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -32599,7 +32678,7 @@
         <v>0.40500000000000003</v>
       </c>
       <c r="F117" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -32619,7 +32698,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="F118" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -32639,7 +32718,7 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="F119" s="14" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -32722,11 +32801,11 @@
       <c r="E124" s="14">
         <v>0.45</v>
       </c>
-      <c r="F124" s="52" t="s">
-        <v>691</v>
+      <c r="F124" s="51" t="s">
+        <v>688</v>
       </c>
       <c r="G124" s="14" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
   </sheetData>
@@ -32752,11 +32831,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="70" t="s">
         <v>372</v>
       </c>
-      <c r="E1" s="73"/>
-      <c r="F1" s="74"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="72"/>
     </row>
     <row r="2" spans="1:6" ht="30">
       <c r="A2" s="14" t="s">
@@ -35138,10 +35217,10 @@
   <dimension ref="A1:L126"/>
   <sheetViews>
     <sheetView zoomScale="57" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18:XFD18"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -35178,7 +35257,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>321</v>
@@ -35187,7 +35266,7 @@
         <v>601</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>364</v>
@@ -35215,19 +35294,19 @@
       <c r="G2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="57" t="s">
+      <c r="H2" s="56" t="s">
         <v>284</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="I2" s="56" t="s">
         <v>284</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="56" t="s">
         <v>604</v>
       </c>
-      <c r="K2" s="57" t="s">
+      <c r="K2" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="57" t="s">
+      <c r="L2" s="56" t="s">
         <v>13</v>
       </c>
     </row>
@@ -36093,19 +36172,19 @@
       <c r="G23" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="H23" s="57" t="s">
+      <c r="H23" s="56" t="s">
         <v>299</v>
       </c>
-      <c r="I23" s="57" t="s">
+      <c r="I23" s="56" t="s">
         <v>309</v>
       </c>
-      <c r="J23" s="57" t="s">
+      <c r="J23" s="56" t="s">
         <v>608</v>
       </c>
-      <c r="K23" s="57" t="s">
+      <c r="K23" s="56" t="s">
         <v>608</v>
       </c>
-      <c r="L23" s="57" t="s">
+      <c r="L23" s="56" t="s">
         <v>381</v>
       </c>
     </row>
@@ -36405,11 +36484,11 @@
       </c>
       <c r="J31" s="14" t="str">
         <f>VLOOKUP(B31,concordance!$B$2:$R$124,15,FALSE)</f>
-        <v>Vegetables and legumes</v>
+        <v>Vegetable oils, nuts and seeds</v>
       </c>
       <c r="K31" s="14" t="str">
         <f>VLOOKUP(B31,concordance!$B$2:$R$124,16,FALSE)</f>
-        <v>Vegetables</v>
+        <v>Vegetable oils, nuts and seeds</v>
       </c>
       <c r="L31" s="14" t="s">
         <v>381</v>
@@ -37742,19 +37821,19 @@
       <c r="G67" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="H67" s="57" t="s">
+      <c r="H67" s="56" t="s">
         <v>298</v>
       </c>
-      <c r="I67" s="57" t="s">
+      <c r="I67" s="56" t="s">
         <v>298</v>
       </c>
-      <c r="J67" s="57" t="s">
+      <c r="J67" s="56" t="s">
         <v>298</v>
       </c>
-      <c r="K67" s="57" t="s">
+      <c r="K67" s="56" t="s">
         <v>298</v>
       </c>
-      <c r="L67" s="57" t="s">
+      <c r="L67" s="56" t="s">
         <v>153</v>
       </c>
     </row>
@@ -37780,19 +37859,19 @@
       <c r="G68" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="H68" s="57" t="s">
+      <c r="H68" s="56" t="s">
         <v>298</v>
       </c>
-      <c r="I68" s="57" t="s">
+      <c r="I68" s="56" t="s">
         <v>298</v>
       </c>
-      <c r="J68" s="57" t="s">
+      <c r="J68" s="56" t="s">
         <v>298</v>
       </c>
-      <c r="K68" s="57" t="s">
+      <c r="K68" s="56" t="s">
         <v>298</v>
       </c>
-      <c r="L68" s="57" t="s">
+      <c r="L68" s="56" t="s">
         <v>153</v>
       </c>
     </row>
@@ -39696,19 +39775,19 @@
       <c r="G123" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="H123" s="57" t="s">
+      <c r="H123" s="56" t="s">
         <v>261</v>
       </c>
-      <c r="I123" s="57" t="s">
+      <c r="I123" s="56" t="s">
         <v>261</v>
       </c>
-      <c r="J123" s="57" t="s">
+      <c r="J123" s="56" t="s">
         <v>607</v>
       </c>
-      <c r="K123" s="57" t="s">
+      <c r="K123" s="56" t="s">
         <v>607</v>
       </c>
-      <c r="L123" s="57" t="s">
+      <c r="L123" s="56" t="s">
         <v>261</v>
       </c>
     </row>

</xml_diff>